<commit_message>
testcase document - added description
</commit_message>
<xml_diff>
--- a/Test Template Document Corp.xlsx
+++ b/Test Template Document Corp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="5468" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="5468" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Project Profile" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
   <si>
     <t>Project ID</t>
   </si>
@@ -149,22 +149,79 @@
     <t>Req No</t>
   </si>
   <si>
-    <t xml:space="preserve">Open EMR Application </t>
-  </si>
-  <si>
-    <t>OP</t>
-  </si>
-  <si>
-    <t>Open EMR</t>
-  </si>
-  <si>
-    <t>Medical Record Management Portal</t>
-  </si>
-  <si>
     <t>Requirement Matrix</t>
   </si>
   <si>
     <t>URL:</t>
+  </si>
+  <si>
+    <t>Orange HRM</t>
+  </si>
+  <si>
+    <t>OH</t>
+  </si>
+  <si>
+    <t>Employee Management Portal</t>
+  </si>
+  <si>
+    <t>Orange HRM Portal</t>
+  </si>
+  <si>
+    <t>Balaji</t>
+  </si>
+  <si>
+    <t>QA Engineer</t>
+  </si>
+  <si>
+    <t>QA Trainer</t>
+  </si>
+  <si>
+    <t>Balaji Dinakaran</t>
+  </si>
+  <si>
+    <t>Smita</t>
+  </si>
+  <si>
+    <t>SC_OH_1</t>
+  </si>
+  <si>
+    <t>OH_Req 3</t>
+  </si>
+  <si>
+    <t>Landing Page</t>
+  </si>
+  <si>
+    <t>SC_OH_2</t>
+  </si>
+  <si>
+    <t>Login Scenario</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Scenaro ID&gt; </t>
+  </si>
+  <si>
+    <t>&lt;Sequence Number&gt;</t>
+  </si>
+  <si>
+    <t>&lt;this specifies the state of the system and environment must be before the specific test case can be run&gt;</t>
+  </si>
+  <si>
+    <t>&lt;This specfies the detailed test steps on how to test.. &gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;Test data used to run by test steps&gt; </t>
+  </si>
+  <si>
+    <t>&lt;decribe the expected result after analysing the requirement&gt;</t>
+  </si>
+  <si>
+    <t>&lt;Mention actual result after execution of the test steps&gt;</t>
+  </si>
+  <si>
+    <t>&lt;status of the test case whether passed or failed or skipped or blocked&gt;</t>
+  </si>
+  <si>
+    <t>&lt;description about the test case&gt;</t>
   </si>
 </sst>
 </file>
@@ -458,7 +515,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -581,6 +638,9 @@
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -623,7 +683,7 @@
         <xdr:cNvPr id="2154" name="Picture 2" descr="pcs">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006A080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006A080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1038,8 +1098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:V18"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7:D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.265625" defaultRowHeight="17.25" customHeight="1"/>
@@ -1055,7 +1115,7 @@
   <sheetData>
     <row r="4" spans="2:4" s="4" customFormat="1" ht="22.5">
       <c r="B4" s="34" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="C4" s="34"/>
       <c r="D4" s="34"/>
@@ -1068,7 +1128,7 @@
         <v>0</v>
       </c>
       <c r="C7" s="35" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D7" s="36"/>
     </row>
@@ -1086,7 +1146,7 @@
         <v>2</v>
       </c>
       <c r="C9" s="37" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D9" s="38"/>
     </row>
@@ -1107,8 +1167,12 @@
       </c>
     </row>
     <row r="13" spans="2:4" ht="13.5">
-      <c r="B13" s="17"/>
-      <c r="C13" s="17"/>
+      <c r="B13" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="17" t="s">
+        <v>42</v>
+      </c>
       <c r="D13" s="11"/>
     </row>
     <row r="14" spans="2:4" ht="17.25" customHeight="1">
@@ -1123,8 +1187,12 @@
       </c>
     </row>
     <row r="15" spans="2:4" ht="13.5">
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
+      <c r="B15" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="17" t="s">
+        <v>43</v>
+      </c>
       <c r="D15" s="11"/>
     </row>
     <row r="16" spans="2:4" ht="17.25" customHeight="1">
@@ -1139,7 +1207,9 @@
       </c>
     </row>
     <row r="17" spans="2:4" ht="13.5">
-      <c r="B17" s="17"/>
+      <c r="B17" s="17" t="s">
+        <v>45</v>
+      </c>
       <c r="C17" s="17"/>
       <c r="D17" s="11"/>
     </row>
@@ -1168,7 +1238,7 @@
   <dimension ref="A2:D18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6:D18"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75"/>
@@ -1181,12 +1251,12 @@
   <sheetData>
     <row r="2" spans="1:4" ht="17.649999999999999">
       <c r="C2" s="16" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="C4" s="18" t="s">
         <v>31</v>
@@ -1211,16 +1281,30 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="15"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
+      <c r="A7" s="42" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="15"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
+      <c r="B8" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D8" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="15"/>
@@ -1297,14 +1381,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L388"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36" defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="18.86328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.1328125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.265625" style="1" customWidth="1"/>
     <col min="3" max="3" width="35.3984375" style="1" customWidth="1"/>
     <col min="4" max="4" width="38.59765625" style="1" customWidth="1"/>
     <col min="5" max="5" width="25.265625" style="1" customWidth="1"/>
@@ -1352,91 +1436,116 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="21" customFormat="1" ht="25.5">
-      <c r="A2" s="33"/>
-      <c r="F2" s="32"/>
-    </row>
-    <row r="3" spans="1:12" s="21" customFormat="1" ht="25.5">
+    <row r="2" spans="1:12" s="21" customFormat="1" ht="75.75" customHeight="1">
+      <c r="A2" s="33" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>59</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E2" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" s="21" customFormat="1">
       <c r="A3" s="33"/>
       <c r="F3" s="32"/>
     </row>
-    <row r="4" spans="1:12" s="21" customFormat="1" ht="25.5">
+    <row r="4" spans="1:12" s="21" customFormat="1">
       <c r="A4" s="33"/>
       <c r="F4" s="32"/>
     </row>
-    <row r="5" spans="1:12" s="21" customFormat="1" ht="25.5">
+    <row r="5" spans="1:12" s="21" customFormat="1">
       <c r="A5" s="33"/>
       <c r="F5" s="32"/>
     </row>
-    <row r="6" spans="1:12" s="21" customFormat="1" ht="25.5">
+    <row r="6" spans="1:12" s="21" customFormat="1">
       <c r="A6" s="33"/>
       <c r="F6" s="32"/>
     </row>
-    <row r="7" spans="1:12" s="21" customFormat="1" ht="25.5">
+    <row r="7" spans="1:12" s="21" customFormat="1">
       <c r="A7" s="33"/>
       <c r="F7" s="32"/>
     </row>
-    <row r="8" spans="1:12" s="21" customFormat="1" ht="25.5">
+    <row r="8" spans="1:12" s="21" customFormat="1">
       <c r="A8" s="33"/>
       <c r="F8" s="32"/>
     </row>
-    <row r="9" spans="1:12" s="21" customFormat="1" ht="25.5">
+    <row r="9" spans="1:12" s="21" customFormat="1">
       <c r="A9" s="33"/>
       <c r="F9" s="32"/>
     </row>
-    <row r="10" spans="1:12" s="21" customFormat="1" ht="25.5">
+    <row r="10" spans="1:12" s="21" customFormat="1">
       <c r="A10" s="33"/>
       <c r="F10" s="32"/>
     </row>
-    <row r="11" spans="1:12" s="21" customFormat="1" ht="25.5">
+    <row r="11" spans="1:12" s="21" customFormat="1">
       <c r="A11" s="33"/>
       <c r="F11" s="32"/>
     </row>
-    <row r="12" spans="1:12" s="21" customFormat="1" ht="25.5">
+    <row r="12" spans="1:12" s="21" customFormat="1">
       <c r="A12" s="33"/>
       <c r="F12" s="32"/>
     </row>
-    <row r="13" spans="1:12" s="21" customFormat="1" ht="25.5">
+    <row r="13" spans="1:12" s="21" customFormat="1">
       <c r="A13" s="33"/>
       <c r="F13" s="32"/>
     </row>
-    <row r="14" spans="1:12" s="21" customFormat="1" ht="25.5">
+    <row r="14" spans="1:12" s="21" customFormat="1">
       <c r="A14" s="33"/>
       <c r="F14" s="32"/>
     </row>
-    <row r="15" spans="1:12" s="21" customFormat="1" ht="25.5">
+    <row r="15" spans="1:12" s="21" customFormat="1">
       <c r="A15" s="33"/>
       <c r="F15" s="32"/>
     </row>
-    <row r="16" spans="1:12" s="21" customFormat="1" ht="25.5">
+    <row r="16" spans="1:12" s="21" customFormat="1">
       <c r="A16" s="33"/>
       <c r="F16" s="32"/>
     </row>
-    <row r="17" spans="1:6" s="21" customFormat="1" ht="25.5">
+    <row r="17" spans="1:6" s="21" customFormat="1">
       <c r="A17" s="33"/>
       <c r="F17" s="32"/>
     </row>
-    <row r="18" spans="1:6" s="21" customFormat="1" ht="25.5">
+    <row r="18" spans="1:6" s="21" customFormat="1">
       <c r="A18" s="33"/>
       <c r="F18" s="32"/>
     </row>
-    <row r="19" spans="1:6" s="21" customFormat="1" ht="25.5">
+    <row r="19" spans="1:6" s="21" customFormat="1">
       <c r="A19" s="33"/>
       <c r="F19" s="32"/>
     </row>
-    <row r="20" spans="1:6" s="21" customFormat="1" ht="25.5">
+    <row r="20" spans="1:6" s="21" customFormat="1">
       <c r="A20" s="33"/>
       <c r="F20" s="32"/>
     </row>
-    <row r="21" spans="1:6" s="21" customFormat="1" ht="25.5">
+    <row r="21" spans="1:6" s="21" customFormat="1">
       <c r="A21" s="33"/>
       <c r="F21" s="32"/>
     </row>
-    <row r="22" spans="1:6" s="21" customFormat="1" ht="25.5">
+    <row r="22" spans="1:6" s="21" customFormat="1">
       <c r="A22" s="33"/>
       <c r="F22" s="32"/>
     </row>
-    <row r="23" spans="1:6" s="21" customFormat="1" ht="25.5">
+    <row r="23" spans="1:6" s="21" customFormat="1">
       <c r="A23" s="33"/>
       <c r="F23" s="32"/>
     </row>
@@ -1808,12 +1917,12 @@
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I1:I1048576">
-      <formula1>"Pass,Fail,Blocked"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I58">
+      <formula1>"passed,failed,skipped,blocked"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1821,8 +1930,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.3984375" defaultRowHeight="12.75"/>
@@ -1954,7 +2063,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Levels xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">L1</Levels>
+    <Category xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Module Artifact</Category>
+    <FolderName xmlns="952a6df7-b138-4f89-9bc4-e7a874ea3254" xsi:nil="true"/>
+    <Material_x0020_Type xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Extra Material</Material_x0020_Type>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2128,14 +2244,7 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Levels xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">L1</Levels>
-    <Category xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Module Artifact</Category>
-    <FolderName xmlns="952a6df7-b138-4f89-9bc4-e7a874ea3254" xsi:nil="true"/>
-    <Material_x0020_Type xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Extra Material</Material_x0020_Type>
-  </documentManagement>
-</p:properties>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2148,9 +2257,18 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67F96C4C-21BE-4526-9614-87D2A1A52CD5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{812CC0C1-FD42-47A7-BEBF-6413B223EE92}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="952a6df7-b138-4f89-9bc4-e7a874ea3254"/>
+    <ds:schemaRef ds:uri="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2175,12 +2293,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{812CC0C1-FD42-47A7-BEBF-6413B223EE92}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67F96C4C-21BE-4526-9614-87D2A1A52CD5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
-    <ds:schemaRef ds:uri="952a6df7-b138-4f89-9bc4-e7a874ea3254"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
updated 5 scenario-11 testcase
</commit_message>
<xml_diff>
--- a/Test Template Document Corp.xlsx
+++ b/Test Template Document Corp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="5468" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="5468" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project Profile" sheetId="6" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="118">
   <si>
     <t>Project ID</t>
   </si>
@@ -137,9 +137,6 @@
     <t>Test Executed Date</t>
   </si>
   <si>
-    <t>https://demo.openemr.io/b/openemr</t>
-  </si>
-  <si>
     <t xml:space="preserve">Actual Result </t>
   </si>
   <si>
@@ -222,14 +219,220 @@
   </si>
   <si>
     <t>&lt;description about the test case&gt;</t>
+  </si>
+  <si>
+    <t>SC_OH_3</t>
+  </si>
+  <si>
+    <t>SC_OH_4</t>
+  </si>
+  <si>
+    <t>SC_OH_5</t>
+  </si>
+  <si>
+    <t>SC_OH_6</t>
+  </si>
+  <si>
+    <t>SC_OH_7</t>
+  </si>
+  <si>
+    <t>SC_OH_8</t>
+  </si>
+  <si>
+    <t>SC_OH_9</t>
+  </si>
+  <si>
+    <t>SC_OH_10</t>
+  </si>
+  <si>
+    <t>SC_OH_11</t>
+  </si>
+  <si>
+    <t>SC_OH_12</t>
+  </si>
+  <si>
+    <t>OH_Req 4</t>
+  </si>
+  <si>
+    <t>TC_OH_1</t>
+  </si>
+  <si>
+    <t>https://opensource-demo.orangehrmlive.com/index.php/</t>
+  </si>
+  <si>
+    <t>To verify the UI Component in the landing page</t>
+  </si>
+  <si>
+    <t>Navigate/access to the url mentioned in the RTM</t>
+  </si>
+  <si>
+    <t>1. Navigate to the url</t>
+  </si>
+  <si>
+    <t>1. Title should be "OrangeHRM".
+2. OrangeHRM Logo should be present
+3. Textbox for entering username and password
+4. Textbox should contain username and password placeholder.
+5. Login button should be present
+6. Link for "Forgot Your Password?" should be present
+7. OrgangeHRM version should be present as "Orange HRM 4.2"
+8. Copyright detail should be present as "© 2005 - 2022 OrangeHRM, Inc. All rights reserved."
+9. Icon with link for Linkendin, Facebook, Twitter, youtube should be present.</t>
+  </si>
+  <si>
+    <t>Status Comments</t>
+  </si>
+  <si>
+    <t>TC_OH_2</t>
+  </si>
+  <si>
+    <t>1. Navigate to the url
+2. Enter username
+3. Enter password
+4. Click Login</t>
+  </si>
+  <si>
+    <t>Data 1:
+Username: Admin
+Password: admin123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">User should be navigated to the dashboard screen </t>
+  </si>
+  <si>
+    <t>To verify the valid login as a enrolled employee.</t>
+  </si>
+  <si>
+    <t>TC_OH_3</t>
+  </si>
+  <si>
+    <t>To verify the invalid login as a enrolled employee</t>
+  </si>
+  <si>
+    <t>Data 1:
+Username: John
+Password: admin123
+Data 2:
+Username: John
+Password: admin123</t>
+  </si>
+  <si>
+    <t>User should be displayed with error message as "Invalid Credential"</t>
+  </si>
+  <si>
+    <t>TC_OH_4</t>
+  </si>
+  <si>
+    <t>To verify empty username are not allowed to login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data 1:
+Password: admin123
+</t>
+  </si>
+  <si>
+    <t>User should be displayed with error message as "Username cannot be empty"</t>
+  </si>
+  <si>
+    <t>TC_OH_5</t>
+  </si>
+  <si>
+    <t>To verify empty password are not allowed to login</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data 1:
+Username: Admin
+</t>
+  </si>
+  <si>
+    <t>User should be displayed with error message as "Password cannot be empty"</t>
+  </si>
+  <si>
+    <t>Landing Page - Forgot Your Password Link</t>
+  </si>
+  <si>
+    <t>TC_OH_6</t>
+  </si>
+  <si>
+    <t>To verify forgot your password link</t>
+  </si>
+  <si>
+    <t>1. Navigate to the url
+2. Click on "Forgot your password?"</t>
+  </si>
+  <si>
+    <t>User should be navigated to forgor your page.</t>
+  </si>
+  <si>
+    <t>Landing Page - Orange HRM link</t>
+  </si>
+  <si>
+    <t>Landing Page - Social Media Link - Facebook, Twitter, Youtube, Linkedin</t>
+  </si>
+  <si>
+    <t>TC_OH_7</t>
+  </si>
+  <si>
+    <t>TC_OH_8</t>
+  </si>
+  <si>
+    <t>1. Navigate to the url
+2. Click on "Facebook icon" in the bottom of page</t>
+  </si>
+  <si>
+    <t>1. Navigate to the url
+2. Click on "Linkedin icon" in the bottom of page</t>
+  </si>
+  <si>
+    <t>To verify Linkedin link is working fine</t>
+  </si>
+  <si>
+    <t>TC_OH_9</t>
+  </si>
+  <si>
+    <t>To verify Facebook icon link is working fine</t>
+  </si>
+  <si>
+    <t>User should be navigated to Orange HRM profle of facebook in new tab.</t>
+  </si>
+  <si>
+    <t>User should be navigated to Orange HRM profile of linkedin in new tab.</t>
+  </si>
+  <si>
+    <t>TC_OH_10</t>
+  </si>
+  <si>
+    <t>TC_OH_11</t>
+  </si>
+  <si>
+    <t>To verify twitter icon link is working fine</t>
+  </si>
+  <si>
+    <t>To verify youtube icon link is working fine</t>
+  </si>
+  <si>
+    <t>1. Navigate to the url
+2. Click on "Twitter icon" in the bottom of page</t>
+  </si>
+  <si>
+    <t>1. Navigate to the url
+2. Click on "Youtube icon" in the bottom of page</t>
+  </si>
+  <si>
+    <t>User should be navigated to youtube Orange HRM channel in new tab.</t>
+  </si>
+  <si>
+    <t>User should be navigated to Orange HRM profle of twitter in new tab.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="[$-409]mmmm\ d\,\ yyyy;@"/>
+    <numFmt numFmtId="166" formatCode="[$-409]dd\-mmm\-yy;@"/>
+    <numFmt numFmtId="167" formatCode="[$-409]d\-mmm\-yy;@"/>
   </numFmts>
   <fonts count="16">
     <font>
@@ -515,7 +718,7 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -615,6 +818,9 @@
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="4" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -639,8 +845,28 @@
     <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="166" fontId="4" fillId="3" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -683,7 +909,7 @@
         <xdr:cNvPr id="2154" name="Picture 2" descr="pcs">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006A080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006A080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1098,7 +1324,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:V18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C7" sqref="C7:D7"/>
     </sheetView>
   </sheetViews>
@@ -1114,11 +1340,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:4" s="4" customFormat="1" ht="22.5">
-      <c r="B4" s="34" t="s">
-        <v>40</v>
-      </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
+      <c r="B4" s="35" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
     </row>
     <row r="5" spans="2:4" s="5" customFormat="1" ht="15">
       <c r="C5" s="6"/>
@@ -1127,28 +1353,28 @@
       <c r="B7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="35" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="36"/>
+      <c r="C7" s="36" t="s">
+        <v>37</v>
+      </c>
+      <c r="D7" s="37"/>
     </row>
     <row r="8" spans="2:4" ht="17.25" customHeight="1">
       <c r="B8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="35" t="s">
-        <v>37</v>
-      </c>
-      <c r="D8" s="36"/>
+      <c r="C8" s="36" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="37"/>
     </row>
     <row r="9" spans="2:4" ht="31.5" customHeight="1">
       <c r="B9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="37" t="s">
-        <v>39</v>
-      </c>
-      <c r="D9" s="38"/>
+      <c r="C9" s="38" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="39"/>
     </row>
     <row r="10" spans="2:4" ht="17.25" customHeight="1">
       <c r="B10" s="9"/>
@@ -1168,12 +1394,14 @@
     </row>
     <row r="13" spans="2:4" ht="13.5">
       <c r="B13" s="17" t="s">
+        <v>40</v>
+      </c>
+      <c r="C13" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="C13" s="17" t="s">
-        <v>42</v>
-      </c>
-      <c r="D13" s="11"/>
+      <c r="D13" s="43">
+        <v>44607</v>
+      </c>
     </row>
     <row r="14" spans="2:4" ht="17.25" customHeight="1">
       <c r="B14" s="10" t="s">
@@ -1188,10 +1416,10 @@
     </row>
     <row r="15" spans="2:4" ht="13.5">
       <c r="B15" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D15" s="11"/>
     </row>
@@ -1208,7 +1436,7 @@
     </row>
     <row r="17" spans="2:4" ht="13.5">
       <c r="B17" s="17" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C17" s="17"/>
       <c r="D17" s="11"/>
@@ -1237,8 +1465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75"/>
@@ -1251,15 +1479,15 @@
   <sheetData>
     <row r="2" spans="1:4" ht="17.649999999999999">
       <c r="C2" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="B4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>31</v>
+        <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="1" customFormat="1" ht="13.15">
@@ -1268,7 +1496,7 @@
     </row>
     <row r="6" spans="1:4" ht="15">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>
@@ -1281,88 +1509,122 @@
       </c>
     </row>
     <row r="7" spans="1:4">
-      <c r="A7" s="42" t="s">
+      <c r="A7" s="34" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="44" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="15" t="s">
         <v>47</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" s="15" t="s">
-        <v>48</v>
       </c>
       <c r="D7" s="15">
         <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:4">
-      <c r="A8" s="15"/>
-      <c r="B8" s="15" t="s">
+      <c r="A8" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="B8" s="44" t="s">
+        <v>48</v>
+      </c>
+      <c r="C8" s="15" t="s">
         <v>49</v>
-      </c>
-      <c r="C8" s="15" t="s">
-        <v>50</v>
       </c>
       <c r="D8" s="15">
         <v>4</v>
       </c>
     </row>
     <row r="9" spans="1:4">
-      <c r="A9" s="15"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
+      <c r="A9" s="34"/>
+      <c r="B9" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" s="44" t="s">
+        <v>94</v>
+      </c>
+      <c r="D9" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="10" spans="1:4">
-      <c r="A10" s="15"/>
-      <c r="B10" s="15"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="15"/>
+      <c r="A10" s="34"/>
+      <c r="B10" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C10" s="44" t="s">
+        <v>99</v>
+      </c>
+      <c r="D10" s="15">
+        <v>1</v>
+      </c>
     </row>
     <row r="11" spans="1:4">
-      <c r="A11" s="15"/>
-      <c r="B11" s="15"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="15"/>
+      <c r="A11" s="34"/>
+      <c r="B11" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="44" t="s">
+        <v>100</v>
+      </c>
+      <c r="D11" s="15">
+        <v>4</v>
+      </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
+      <c r="B12" s="15" t="s">
+        <v>62</v>
+      </c>
       <c r="C12" s="15"/>
       <c r="D12" s="15"/>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="15"/>
-      <c r="B13" s="15"/>
+      <c r="B13" s="15" t="s">
+        <v>63</v>
+      </c>
       <c r="C13" s="15"/>
       <c r="D13" s="15"/>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
+      <c r="B14" s="15" t="s">
+        <v>64</v>
+      </c>
       <c r="C14" s="15"/>
       <c r="D14" s="15"/>
     </row>
     <row r="15" spans="1:4" ht="13.9">
       <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
+      <c r="B15" s="15" t="s">
+        <v>65</v>
+      </c>
       <c r="C15" s="15"/>
       <c r="D15" s="31"/>
     </row>
     <row r="16" spans="1:4" ht="13.9">
       <c r="A16" s="15"/>
-      <c r="B16" s="15"/>
+      <c r="B16" s="15" t="s">
+        <v>66</v>
+      </c>
       <c r="C16" s="15"/>
       <c r="D16" s="31"/>
     </row>
     <row r="17" spans="1:4" ht="13.9">
       <c r="A17" s="15"/>
-      <c r="B17" s="15"/>
+      <c r="B17" s="15" t="s">
+        <v>67</v>
+      </c>
       <c r="C17" s="15"/>
       <c r="D17" s="31"/>
     </row>
     <row r="18" spans="1:4" ht="13.9">
       <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
+      <c r="B18" s="15" t="s">
+        <v>68</v>
+      </c>
       <c r="C18" s="15"/>
       <c r="D18" s="31"/>
     </row>
@@ -1379,10 +1641,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L388"/>
+  <dimension ref="A1:M388"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36" defaultRowHeight="12.75"/>
@@ -1393,12 +1655,13 @@
     <col min="4" max="4" width="38.59765625" style="1" customWidth="1"/>
     <col min="5" max="5" width="25.265625" style="1" customWidth="1"/>
     <col min="6" max="6" width="33.73046875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="35.59765625" style="1" customWidth="1"/>
-    <col min="8" max="9" width="26.1328125" style="1" customWidth="1"/>
-    <col min="10" max="16384" width="36" style="1"/>
+    <col min="7" max="7" width="57.9296875" style="1" customWidth="1"/>
+    <col min="8" max="10" width="26.1328125" style="1" customWidth="1"/>
+    <col min="11" max="11" width="36" style="49"/>
+    <col min="12" max="16384" width="36" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="20" customFormat="1">
+    <row r="1" spans="1:13" s="20" customFormat="1">
       <c r="A1" s="19" t="s">
         <v>14</v>
       </c>
@@ -1421,506 +1684,1466 @@
         <v>19</v>
       </c>
       <c r="H1" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="I1" s="19" t="s">
         <v>32</v>
       </c>
-      <c r="I1" s="19" t="s">
-        <v>33</v>
-      </c>
-      <c r="J1" s="19" t="s">
+      <c r="J1" s="46" t="s">
+        <v>76</v>
+      </c>
+      <c r="K1" s="47" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="L1" s="19" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="M1" s="19" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:12" s="21" customFormat="1" ht="75.75" customHeight="1">
+    <row r="2" spans="1:13" s="21" customFormat="1" ht="51.4" customHeight="1">
       <c r="A2" s="33" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="C2" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="E2" s="21" t="s">
+        <v>53</v>
+      </c>
+      <c r="F2" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="H2" s="21" t="s">
+        <v>56</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>57</v>
+      </c>
+      <c r="K2" s="48"/>
+    </row>
+    <row r="3" spans="1:13" s="21" customFormat="1" ht="113.65" customHeight="1">
+      <c r="A3" s="33" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="45" t="s">
+        <v>70</v>
+      </c>
+      <c r="C3" s="45" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="E3" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="F3" s="32"/>
+      <c r="G3" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="K3" s="48">
+        <v>44607</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" s="21" customFormat="1" ht="45.75" customHeight="1">
+      <c r="A4" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="45" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="E4" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="F4" s="50" t="s">
+        <v>79</v>
+      </c>
+      <c r="G4" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" s="48">
+        <v>44607</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" s="21" customFormat="1" ht="121.5" customHeight="1">
+      <c r="A5" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B5" s="45" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="45" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="E5" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="G5" s="45" t="s">
+        <v>85</v>
+      </c>
+      <c r="K5" s="48">
+        <v>44607</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" s="21" customFormat="1" ht="121.5" customHeight="1">
+      <c r="A6" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B6" s="45" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" s="45" t="s">
+        <v>87</v>
+      </c>
+      <c r="D6" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="E6" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="50" t="s">
+        <v>88</v>
+      </c>
+      <c r="G6" s="45" t="s">
+        <v>89</v>
+      </c>
+      <c r="K6" s="48">
+        <v>44607</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" s="21" customFormat="1" ht="121.5" customHeight="1">
+      <c r="A7" s="33" t="s">
+        <v>48</v>
+      </c>
+      <c r="B7" s="45" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="45" t="s">
+        <v>91</v>
+      </c>
+      <c r="D7" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="E7" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="F7" s="50" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="45" t="s">
+        <v>93</v>
+      </c>
+      <c r="K7" s="48">
+        <v>44607</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" s="21" customFormat="1" ht="121.5" customHeight="1">
+      <c r="A8" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="D2" s="21" t="s">
-        <v>53</v>
-      </c>
-      <c r="E2" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="F2" s="32" t="s">
-        <v>55</v>
-      </c>
-      <c r="G2" s="21" t="s">
-        <v>56</v>
-      </c>
-      <c r="H2" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="I2" s="21" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" s="21" customFormat="1">
-      <c r="A3" s="33"/>
-      <c r="F3" s="32"/>
-    </row>
-    <row r="4" spans="1:12" s="21" customFormat="1">
-      <c r="A4" s="33"/>
-      <c r="F4" s="32"/>
-    </row>
-    <row r="5" spans="1:12" s="21" customFormat="1">
-      <c r="A5" s="33"/>
-      <c r="F5" s="32"/>
-    </row>
-    <row r="6" spans="1:12" s="21" customFormat="1">
-      <c r="A6" s="33"/>
-      <c r="F6" s="32"/>
-    </row>
-    <row r="7" spans="1:12" s="21" customFormat="1">
-      <c r="A7" s="33"/>
-      <c r="F7" s="32"/>
-    </row>
-    <row r="8" spans="1:12" s="21" customFormat="1">
-      <c r="A8" s="33"/>
-      <c r="F8" s="32"/>
-    </row>
-    <row r="9" spans="1:12" s="21" customFormat="1">
-      <c r="A9" s="33"/>
+      <c r="B8" s="45" t="s">
+        <v>95</v>
+      </c>
+      <c r="C8" s="45" t="s">
+        <v>96</v>
+      </c>
+      <c r="D8" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="E8" s="45" t="s">
+        <v>97</v>
+      </c>
+      <c r="G8" s="50" t="s">
+        <v>98</v>
+      </c>
+      <c r="K8" s="48"/>
+    </row>
+    <row r="9" spans="1:13" s="21" customFormat="1">
+      <c r="A9" s="33" t="s">
+        <v>60</v>
+      </c>
+      <c r="B9" s="45" t="s">
+        <v>101</v>
+      </c>
       <c r="F9" s="32"/>
-    </row>
-    <row r="10" spans="1:12" s="21" customFormat="1">
-      <c r="A10" s="33"/>
+      <c r="K9" s="48"/>
+    </row>
+    <row r="10" spans="1:13" s="21" customFormat="1" ht="38.25">
+      <c r="A10" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="45" t="s">
+        <v>102</v>
+      </c>
+      <c r="C10" s="45" t="s">
+        <v>105</v>
+      </c>
+      <c r="D10" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" s="45" t="s">
+        <v>104</v>
+      </c>
       <c r="F10" s="32"/>
-    </row>
-    <row r="11" spans="1:12" s="21" customFormat="1">
-      <c r="A11" s="33"/>
+      <c r="G10" s="45" t="s">
+        <v>109</v>
+      </c>
+      <c r="K10" s="48"/>
+    </row>
+    <row r="11" spans="1:13" s="21" customFormat="1" ht="38.25">
+      <c r="A11" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B11" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11" s="45" t="s">
+        <v>107</v>
+      </c>
+      <c r="D11" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="45" t="s">
+        <v>103</v>
+      </c>
       <c r="F11" s="32"/>
-    </row>
-    <row r="12" spans="1:12" s="21" customFormat="1">
-      <c r="A12" s="33"/>
+      <c r="G11" s="45" t="s">
+        <v>108</v>
+      </c>
+      <c r="K11" s="48"/>
+    </row>
+    <row r="12" spans="1:13" s="21" customFormat="1" ht="38.25">
+      <c r="A12" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="45" t="s">
+        <v>110</v>
+      </c>
+      <c r="C12" s="45" t="s">
+        <v>112</v>
+      </c>
+      <c r="D12" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="E12" s="45" t="s">
+        <v>114</v>
+      </c>
       <c r="F12" s="32"/>
-    </row>
-    <row r="13" spans="1:12" s="21" customFormat="1">
-      <c r="A13" s="33"/>
+      <c r="G12" s="45" t="s">
+        <v>117</v>
+      </c>
+      <c r="K12" s="48"/>
+    </row>
+    <row r="13" spans="1:13" s="21" customFormat="1" ht="38.25">
+      <c r="A13" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B13" s="45" t="s">
+        <v>111</v>
+      </c>
+      <c r="C13" s="45" t="s">
+        <v>113</v>
+      </c>
+      <c r="D13" s="45" t="s">
+        <v>73</v>
+      </c>
+      <c r="E13" s="45" t="s">
+        <v>115</v>
+      </c>
       <c r="F13" s="32"/>
-    </row>
-    <row r="14" spans="1:12" s="21" customFormat="1">
+      <c r="G13" s="45" t="s">
+        <v>116</v>
+      </c>
+      <c r="K13" s="48"/>
+    </row>
+    <row r="14" spans="1:13" s="21" customFormat="1">
       <c r="A14" s="33"/>
       <c r="F14" s="32"/>
-    </row>
-    <row r="15" spans="1:12" s="21" customFormat="1">
+      <c r="K14" s="48"/>
+    </row>
+    <row r="15" spans="1:13" s="21" customFormat="1">
       <c r="A15" s="33"/>
       <c r="F15" s="32"/>
-    </row>
-    <row r="16" spans="1:12" s="21" customFormat="1">
+      <c r="K15" s="48"/>
+    </row>
+    <row r="16" spans="1:13" s="21" customFormat="1">
       <c r="A16" s="33"/>
       <c r="F16" s="32"/>
-    </row>
-    <row r="17" spans="1:6" s="21" customFormat="1">
+      <c r="K16" s="48"/>
+    </row>
+    <row r="17" spans="1:11" s="21" customFormat="1">
       <c r="A17" s="33"/>
       <c r="F17" s="32"/>
-    </row>
-    <row r="18" spans="1:6" s="21" customFormat="1">
+      <c r="K17" s="48"/>
+    </row>
+    <row r="18" spans="1:11" s="21" customFormat="1">
       <c r="A18" s="33"/>
       <c r="F18" s="32"/>
-    </row>
-    <row r="19" spans="1:6" s="21" customFormat="1">
+      <c r="K18" s="48"/>
+    </row>
+    <row r="19" spans="1:11" s="21" customFormat="1">
       <c r="A19" s="33"/>
       <c r="F19" s="32"/>
-    </row>
-    <row r="20" spans="1:6" s="21" customFormat="1">
-      <c r="A20" s="33"/>
+      <c r="K19" s="48"/>
+    </row>
+    <row r="20" spans="1:11" s="21" customFormat="1">
       <c r="F20" s="32"/>
-    </row>
-    <row r="21" spans="1:6" s="21" customFormat="1">
-      <c r="A21" s="33"/>
+      <c r="K20" s="48"/>
+    </row>
+    <row r="21" spans="1:11" s="21" customFormat="1">
       <c r="F21" s="32"/>
-    </row>
-    <row r="22" spans="1:6" s="21" customFormat="1">
-      <c r="A22" s="33"/>
+      <c r="K21" s="48"/>
+    </row>
+    <row r="22" spans="1:11" s="21" customFormat="1">
       <c r="F22" s="32"/>
-    </row>
-    <row r="23" spans="1:6" s="21" customFormat="1">
-      <c r="A23" s="33"/>
+      <c r="K22" s="48"/>
+    </row>
+    <row r="23" spans="1:11" s="21" customFormat="1">
       <c r="F23" s="32"/>
-    </row>
-    <row r="24" spans="1:6" s="21" customFormat="1"/>
-    <row r="25" spans="1:6" s="21" customFormat="1"/>
-    <row r="26" spans="1:6" s="21" customFormat="1"/>
-    <row r="27" spans="1:6" s="21" customFormat="1"/>
-    <row r="28" spans="1:6" s="21" customFormat="1"/>
-    <row r="29" spans="1:6" s="21" customFormat="1"/>
-    <row r="30" spans="1:6" s="21" customFormat="1"/>
-    <row r="31" spans="1:6" s="21" customFormat="1"/>
-    <row r="32" spans="1:6" s="21" customFormat="1"/>
-    <row r="33" s="21" customFormat="1"/>
-    <row r="34" s="21" customFormat="1"/>
-    <row r="35" s="21" customFormat="1"/>
-    <row r="36" s="21" customFormat="1"/>
-    <row r="37" s="21" customFormat="1"/>
-    <row r="38" s="21" customFormat="1"/>
-    <row r="39" s="21" customFormat="1"/>
-    <row r="40" s="21" customFormat="1"/>
-    <row r="41" s="21" customFormat="1"/>
-    <row r="42" s="21" customFormat="1"/>
-    <row r="43" s="21" customFormat="1"/>
-    <row r="44" s="21" customFormat="1"/>
-    <row r="45" s="21" customFormat="1"/>
-    <row r="46" s="21" customFormat="1"/>
-    <row r="47" s="21" customFormat="1"/>
-    <row r="48" s="21" customFormat="1"/>
-    <row r="49" s="21" customFormat="1"/>
-    <row r="50" s="21" customFormat="1"/>
-    <row r="51" s="21" customFormat="1"/>
-    <row r="52" s="21" customFormat="1"/>
-    <row r="53" s="21" customFormat="1"/>
-    <row r="54" s="21" customFormat="1"/>
-    <row r="55" s="21" customFormat="1"/>
-    <row r="56" s="21" customFormat="1"/>
-    <row r="57" s="21" customFormat="1"/>
-    <row r="58" s="21" customFormat="1"/>
-    <row r="59" s="21" customFormat="1"/>
-    <row r="60" s="21" customFormat="1"/>
-    <row r="61" s="21" customFormat="1"/>
-    <row r="62" s="21" customFormat="1"/>
-    <row r="63" s="21" customFormat="1"/>
-    <row r="64" s="21" customFormat="1"/>
-    <row r="65" s="21" customFormat="1"/>
-    <row r="66" s="21" customFormat="1"/>
-    <row r="67" s="21" customFormat="1"/>
-    <row r="68" s="21" customFormat="1"/>
-    <row r="69" s="21" customFormat="1"/>
-    <row r="70" s="21" customFormat="1"/>
-    <row r="71" s="21" customFormat="1"/>
-    <row r="72" s="21" customFormat="1"/>
-    <row r="73" s="21" customFormat="1"/>
-    <row r="74" s="21" customFormat="1"/>
-    <row r="75" s="21" customFormat="1"/>
-    <row r="76" s="21" customFormat="1"/>
-    <row r="77" s="21" customFormat="1"/>
-    <row r="78" s="21" customFormat="1"/>
-    <row r="79" s="21" customFormat="1"/>
-    <row r="80" s="21" customFormat="1"/>
-    <row r="81" s="21" customFormat="1"/>
-    <row r="82" s="21" customFormat="1"/>
-    <row r="83" s="21" customFormat="1"/>
-    <row r="84" s="21" customFormat="1"/>
-    <row r="85" s="21" customFormat="1"/>
-    <row r="86" s="21" customFormat="1"/>
-    <row r="87" s="21" customFormat="1"/>
-    <row r="88" s="21" customFormat="1"/>
-    <row r="89" s="21" customFormat="1"/>
-    <row r="90" s="21" customFormat="1"/>
-    <row r="91" s="21" customFormat="1"/>
-    <row r="92" s="21" customFormat="1"/>
-    <row r="93" s="21" customFormat="1"/>
-    <row r="94" s="21" customFormat="1"/>
-    <row r="95" s="21" customFormat="1"/>
-    <row r="96" s="21" customFormat="1"/>
-    <row r="97" s="21" customFormat="1"/>
-    <row r="98" s="21" customFormat="1"/>
-    <row r="99" s="21" customFormat="1"/>
-    <row r="100" s="21" customFormat="1"/>
-    <row r="101" s="21" customFormat="1"/>
-    <row r="102" s="21" customFormat="1"/>
-    <row r="103" s="21" customFormat="1"/>
-    <row r="104" s="21" customFormat="1"/>
-    <row r="105" s="21" customFormat="1"/>
-    <row r="106" s="21" customFormat="1"/>
-    <row r="107" s="21" customFormat="1"/>
-    <row r="108" s="21" customFormat="1"/>
-    <row r="109" s="21" customFormat="1"/>
-    <row r="110" s="21" customFormat="1"/>
-    <row r="111" s="21" customFormat="1"/>
-    <row r="112" s="21" customFormat="1"/>
-    <row r="113" s="21" customFormat="1"/>
-    <row r="114" s="21" customFormat="1"/>
-    <row r="115" s="21" customFormat="1"/>
-    <row r="116" s="21" customFormat="1"/>
-    <row r="117" s="21" customFormat="1"/>
-    <row r="118" s="21" customFormat="1"/>
-    <row r="119" s="21" customFormat="1"/>
-    <row r="120" s="21" customFormat="1"/>
-    <row r="121" s="21" customFormat="1"/>
-    <row r="122" s="21" customFormat="1"/>
-    <row r="123" s="21" customFormat="1"/>
-    <row r="124" s="21" customFormat="1"/>
-    <row r="125" s="21" customFormat="1"/>
-    <row r="126" s="21" customFormat="1"/>
-    <row r="127" s="21" customFormat="1"/>
-    <row r="128" s="21" customFormat="1"/>
-    <row r="129" s="21" customFormat="1"/>
-    <row r="130" s="21" customFormat="1"/>
-    <row r="131" s="21" customFormat="1"/>
-    <row r="132" s="21" customFormat="1"/>
-    <row r="133" s="21" customFormat="1"/>
-    <row r="134" s="21" customFormat="1"/>
-    <row r="135" s="21" customFormat="1"/>
-    <row r="136" s="21" customFormat="1"/>
-    <row r="137" s="21" customFormat="1"/>
-    <row r="138" s="21" customFormat="1"/>
-    <row r="139" s="21" customFormat="1"/>
-    <row r="140" s="21" customFormat="1"/>
-    <row r="141" s="21" customFormat="1"/>
-    <row r="142" s="21" customFormat="1"/>
-    <row r="143" s="21" customFormat="1"/>
-    <row r="144" s="21" customFormat="1"/>
-    <row r="145" s="21" customFormat="1"/>
-    <row r="146" s="21" customFormat="1"/>
-    <row r="147" s="21" customFormat="1"/>
-    <row r="148" s="21" customFormat="1"/>
-    <row r="149" s="21" customFormat="1"/>
-    <row r="150" s="21" customFormat="1"/>
-    <row r="151" s="21" customFormat="1"/>
-    <row r="152" s="21" customFormat="1"/>
-    <row r="153" s="21" customFormat="1"/>
-    <row r="154" s="21" customFormat="1"/>
-    <row r="155" s="21" customFormat="1"/>
-    <row r="156" s="21" customFormat="1"/>
-    <row r="157" s="21" customFormat="1"/>
-    <row r="158" s="21" customFormat="1"/>
-    <row r="159" s="21" customFormat="1"/>
-    <row r="160" s="21" customFormat="1"/>
-    <row r="161" s="21" customFormat="1"/>
-    <row r="162" s="21" customFormat="1"/>
-    <row r="163" s="21" customFormat="1"/>
-    <row r="164" s="21" customFormat="1"/>
-    <row r="165" s="21" customFormat="1"/>
-    <row r="166" s="21" customFormat="1"/>
-    <row r="167" s="21" customFormat="1"/>
-    <row r="168" s="21" customFormat="1"/>
-    <row r="169" s="21" customFormat="1"/>
-    <row r="170" s="21" customFormat="1"/>
-    <row r="171" s="21" customFormat="1"/>
-    <row r="172" s="21" customFormat="1"/>
-    <row r="173" s="21" customFormat="1"/>
-    <row r="174" s="21" customFormat="1"/>
-    <row r="175" s="21" customFormat="1"/>
-    <row r="176" s="21" customFormat="1"/>
-    <row r="177" s="21" customFormat="1"/>
-    <row r="178" s="21" customFormat="1"/>
-    <row r="179" s="21" customFormat="1"/>
-    <row r="180" s="21" customFormat="1"/>
-    <row r="181" s="21" customFormat="1"/>
-    <row r="182" s="21" customFormat="1"/>
-    <row r="183" s="21" customFormat="1"/>
-    <row r="184" s="21" customFormat="1"/>
-    <row r="185" s="21" customFormat="1"/>
-    <row r="186" s="21" customFormat="1"/>
-    <row r="187" s="21" customFormat="1"/>
-    <row r="188" s="21" customFormat="1"/>
-    <row r="189" s="21" customFormat="1"/>
-    <row r="190" s="21" customFormat="1"/>
-    <row r="191" s="21" customFormat="1"/>
-    <row r="192" s="21" customFormat="1"/>
-    <row r="193" s="21" customFormat="1"/>
-    <row r="194" s="21" customFormat="1"/>
-    <row r="195" s="21" customFormat="1"/>
-    <row r="196" s="21" customFormat="1"/>
-    <row r="197" s="21" customFormat="1"/>
-    <row r="198" s="21" customFormat="1"/>
-    <row r="199" s="21" customFormat="1"/>
-    <row r="200" s="21" customFormat="1"/>
-    <row r="201" s="21" customFormat="1"/>
-    <row r="202" s="21" customFormat="1"/>
-    <row r="203" s="21" customFormat="1"/>
-    <row r="204" s="21" customFormat="1"/>
-    <row r="205" s="21" customFormat="1"/>
-    <row r="206" s="21" customFormat="1"/>
-    <row r="207" s="21" customFormat="1"/>
-    <row r="208" s="21" customFormat="1"/>
-    <row r="209" s="21" customFormat="1"/>
-    <row r="210" s="21" customFormat="1"/>
-    <row r="211" s="21" customFormat="1"/>
-    <row r="212" s="21" customFormat="1"/>
-    <row r="213" s="21" customFormat="1"/>
-    <row r="214" s="21" customFormat="1"/>
-    <row r="215" s="21" customFormat="1"/>
-    <row r="216" s="21" customFormat="1"/>
-    <row r="217" s="21" customFormat="1"/>
-    <row r="218" s="21" customFormat="1"/>
-    <row r="219" s="21" customFormat="1"/>
-    <row r="220" s="21" customFormat="1"/>
-    <row r="221" s="21" customFormat="1"/>
-    <row r="222" s="21" customFormat="1"/>
-    <row r="223" s="21" customFormat="1"/>
-    <row r="224" s="21" customFormat="1"/>
-    <row r="225" s="21" customFormat="1"/>
-    <row r="226" s="21" customFormat="1"/>
-    <row r="227" s="21" customFormat="1"/>
-    <row r="228" s="21" customFormat="1"/>
-    <row r="229" s="21" customFormat="1"/>
-    <row r="230" s="21" customFormat="1"/>
-    <row r="231" s="21" customFormat="1"/>
-    <row r="232" s="21" customFormat="1"/>
-    <row r="233" s="21" customFormat="1"/>
-    <row r="234" s="21" customFormat="1"/>
-    <row r="235" s="21" customFormat="1"/>
-    <row r="236" s="21" customFormat="1"/>
-    <row r="237" s="21" customFormat="1"/>
-    <row r="238" s="21" customFormat="1"/>
-    <row r="239" s="21" customFormat="1"/>
-    <row r="240" s="21" customFormat="1"/>
-    <row r="241" s="21" customFormat="1"/>
-    <row r="242" s="21" customFormat="1"/>
-    <row r="243" s="21" customFormat="1"/>
-    <row r="244" s="21" customFormat="1"/>
-    <row r="245" s="21" customFormat="1"/>
-    <row r="246" s="21" customFormat="1"/>
-    <row r="247" s="21" customFormat="1"/>
-    <row r="248" s="21" customFormat="1"/>
-    <row r="249" s="21" customFormat="1"/>
-    <row r="250" s="21" customFormat="1"/>
-    <row r="251" s="21" customFormat="1"/>
-    <row r="252" s="21" customFormat="1"/>
-    <row r="253" s="21" customFormat="1"/>
-    <row r="254" s="21" customFormat="1"/>
-    <row r="255" s="21" customFormat="1"/>
-    <row r="256" s="21" customFormat="1"/>
-    <row r="257" s="21" customFormat="1"/>
-    <row r="258" s="21" customFormat="1"/>
-    <row r="259" s="21" customFormat="1"/>
-    <row r="260" s="21" customFormat="1"/>
-    <row r="261" s="21" customFormat="1"/>
-    <row r="262" s="21" customFormat="1"/>
-    <row r="263" s="21" customFormat="1"/>
-    <row r="264" s="21" customFormat="1"/>
-    <row r="265" s="21" customFormat="1"/>
-    <row r="266" s="21" customFormat="1"/>
-    <row r="267" s="21" customFormat="1"/>
-    <row r="268" s="21" customFormat="1"/>
-    <row r="269" s="21" customFormat="1"/>
-    <row r="270" s="21" customFormat="1"/>
-    <row r="271" s="21" customFormat="1"/>
-    <row r="272" s="21" customFormat="1"/>
-    <row r="273" s="21" customFormat="1"/>
-    <row r="274" s="21" customFormat="1"/>
-    <row r="275" s="21" customFormat="1"/>
-    <row r="276" s="21" customFormat="1"/>
-    <row r="277" s="21" customFormat="1"/>
-    <row r="278" s="21" customFormat="1"/>
-    <row r="279" s="21" customFormat="1"/>
-    <row r="280" s="21" customFormat="1"/>
-    <row r="281" s="21" customFormat="1"/>
-    <row r="282" s="21" customFormat="1"/>
-    <row r="283" s="21" customFormat="1"/>
-    <row r="284" s="21" customFormat="1"/>
-    <row r="285" s="21" customFormat="1"/>
-    <row r="286" s="21" customFormat="1"/>
-    <row r="287" s="21" customFormat="1"/>
-    <row r="288" s="21" customFormat="1"/>
-    <row r="289" s="21" customFormat="1"/>
-    <row r="290" s="21" customFormat="1"/>
-    <row r="291" s="21" customFormat="1"/>
-    <row r="292" s="21" customFormat="1"/>
-    <row r="293" s="21" customFormat="1"/>
-    <row r="294" s="21" customFormat="1"/>
-    <row r="295" s="21" customFormat="1"/>
-    <row r="296" s="21" customFormat="1"/>
-    <row r="297" s="21" customFormat="1"/>
-    <row r="298" s="21" customFormat="1"/>
-    <row r="299" s="21" customFormat="1"/>
-    <row r="300" s="21" customFormat="1"/>
-    <row r="301" s="21" customFormat="1"/>
-    <row r="302" s="21" customFormat="1"/>
-    <row r="303" s="21" customFormat="1"/>
-    <row r="304" s="21" customFormat="1"/>
-    <row r="305" s="21" customFormat="1"/>
-    <row r="306" s="21" customFormat="1"/>
-    <row r="307" s="21" customFormat="1"/>
-    <row r="308" s="21" customFormat="1"/>
-    <row r="309" s="21" customFormat="1"/>
-    <row r="310" s="21" customFormat="1"/>
-    <row r="311" s="21" customFormat="1"/>
-    <row r="312" s="21" customFormat="1"/>
-    <row r="313" s="21" customFormat="1"/>
-    <row r="314" s="21" customFormat="1"/>
-    <row r="315" s="21" customFormat="1"/>
-    <row r="316" s="21" customFormat="1"/>
-    <row r="317" s="21" customFormat="1"/>
-    <row r="318" s="21" customFormat="1"/>
-    <row r="319" s="21" customFormat="1"/>
-    <row r="320" s="21" customFormat="1"/>
-    <row r="321" s="21" customFormat="1"/>
-    <row r="322" s="21" customFormat="1"/>
-    <row r="323" s="21" customFormat="1"/>
-    <row r="324" s="21" customFormat="1"/>
-    <row r="325" s="21" customFormat="1"/>
-    <row r="326" s="21" customFormat="1"/>
-    <row r="327" s="21" customFormat="1"/>
-    <row r="328" s="21" customFormat="1"/>
-    <row r="329" s="21" customFormat="1"/>
-    <row r="330" s="21" customFormat="1"/>
-    <row r="331" s="21" customFormat="1"/>
-    <row r="332" s="21" customFormat="1"/>
-    <row r="333" s="21" customFormat="1"/>
-    <row r="334" s="21" customFormat="1"/>
-    <row r="335" s="21" customFormat="1"/>
-    <row r="336" s="21" customFormat="1"/>
-    <row r="337" s="21" customFormat="1"/>
-    <row r="338" s="21" customFormat="1"/>
-    <row r="339" s="21" customFormat="1"/>
-    <row r="340" s="21" customFormat="1"/>
-    <row r="341" s="21" customFormat="1"/>
-    <row r="342" s="21" customFormat="1"/>
-    <row r="343" s="21" customFormat="1"/>
-    <row r="344" s="21" customFormat="1"/>
-    <row r="345" s="21" customFormat="1"/>
-    <row r="346" s="21" customFormat="1"/>
-    <row r="347" s="21" customFormat="1"/>
-    <row r="348" s="21" customFormat="1"/>
-    <row r="349" s="21" customFormat="1"/>
-    <row r="350" s="21" customFormat="1"/>
-    <row r="351" s="21" customFormat="1"/>
-    <row r="352" s="21" customFormat="1"/>
-    <row r="353" s="21" customFormat="1"/>
-    <row r="354" s="21" customFormat="1"/>
-    <row r="355" s="21" customFormat="1"/>
-    <row r="356" s="21" customFormat="1"/>
-    <row r="357" s="21" customFormat="1"/>
-    <row r="358" s="21" customFormat="1"/>
-    <row r="359" s="21" customFormat="1"/>
-    <row r="360" s="21" customFormat="1"/>
-    <row r="361" s="21" customFormat="1"/>
-    <row r="362" s="21" customFormat="1"/>
-    <row r="363" s="21" customFormat="1"/>
-    <row r="364" s="21" customFormat="1"/>
-    <row r="365" s="21" customFormat="1"/>
-    <row r="366" s="21" customFormat="1"/>
-    <row r="367" s="21" customFormat="1"/>
-    <row r="368" s="21" customFormat="1"/>
-    <row r="369" s="21" customFormat="1"/>
-    <row r="370" s="21" customFormat="1"/>
-    <row r="371" s="21" customFormat="1"/>
-    <row r="372" s="21" customFormat="1"/>
-    <row r="373" s="21" customFormat="1"/>
-    <row r="374" s="21" customFormat="1"/>
-    <row r="375" s="21" customFormat="1"/>
-    <row r="376" s="21" customFormat="1"/>
-    <row r="377" s="21" customFormat="1"/>
-    <row r="378" s="21" customFormat="1"/>
-    <row r="379" s="21" customFormat="1"/>
-    <row r="380" s="21" customFormat="1"/>
-    <row r="381" s="21" customFormat="1"/>
-    <row r="382" s="21" customFormat="1"/>
-    <row r="383" s="21" customFormat="1"/>
-    <row r="384" s="21" customFormat="1"/>
-    <row r="385" s="21" customFormat="1"/>
-    <row r="386" s="21" customFormat="1"/>
-    <row r="387" s="21" customFormat="1"/>
-    <row r="388" s="21" customFormat="1"/>
+      <c r="K23" s="48"/>
+    </row>
+    <row r="24" spans="1:11" s="21" customFormat="1">
+      <c r="K24" s="48"/>
+    </row>
+    <row r="25" spans="1:11" s="21" customFormat="1">
+      <c r="K25" s="48"/>
+    </row>
+    <row r="26" spans="1:11" s="21" customFormat="1">
+      <c r="K26" s="48"/>
+    </row>
+    <row r="27" spans="1:11" s="21" customFormat="1">
+      <c r="K27" s="48"/>
+    </row>
+    <row r="28" spans="1:11" s="21" customFormat="1">
+      <c r="K28" s="48"/>
+    </row>
+    <row r="29" spans="1:11" s="21" customFormat="1">
+      <c r="K29" s="48"/>
+    </row>
+    <row r="30" spans="1:11" s="21" customFormat="1">
+      <c r="K30" s="48"/>
+    </row>
+    <row r="31" spans="1:11" s="21" customFormat="1">
+      <c r="K31" s="48"/>
+    </row>
+    <row r="32" spans="1:11" s="21" customFormat="1">
+      <c r="K32" s="48"/>
+    </row>
+    <row r="33" spans="11:11" s="21" customFormat="1">
+      <c r="K33" s="48"/>
+    </row>
+    <row r="34" spans="11:11" s="21" customFormat="1">
+      <c r="K34" s="48"/>
+    </row>
+    <row r="35" spans="11:11" s="21" customFormat="1">
+      <c r="K35" s="48"/>
+    </row>
+    <row r="36" spans="11:11" s="21" customFormat="1">
+      <c r="K36" s="48"/>
+    </row>
+    <row r="37" spans="11:11" s="21" customFormat="1">
+      <c r="K37" s="48"/>
+    </row>
+    <row r="38" spans="11:11" s="21" customFormat="1">
+      <c r="K38" s="48"/>
+    </row>
+    <row r="39" spans="11:11" s="21" customFormat="1">
+      <c r="K39" s="48"/>
+    </row>
+    <row r="40" spans="11:11" s="21" customFormat="1">
+      <c r="K40" s="48"/>
+    </row>
+    <row r="41" spans="11:11" s="21" customFormat="1">
+      <c r="K41" s="48"/>
+    </row>
+    <row r="42" spans="11:11" s="21" customFormat="1">
+      <c r="K42" s="48"/>
+    </row>
+    <row r="43" spans="11:11" s="21" customFormat="1">
+      <c r="K43" s="48"/>
+    </row>
+    <row r="44" spans="11:11" s="21" customFormat="1">
+      <c r="K44" s="48"/>
+    </row>
+    <row r="45" spans="11:11" s="21" customFormat="1">
+      <c r="K45" s="48"/>
+    </row>
+    <row r="46" spans="11:11" s="21" customFormat="1">
+      <c r="K46" s="48"/>
+    </row>
+    <row r="47" spans="11:11" s="21" customFormat="1">
+      <c r="K47" s="48"/>
+    </row>
+    <row r="48" spans="11:11" s="21" customFormat="1">
+      <c r="K48" s="48"/>
+    </row>
+    <row r="49" spans="11:11" s="21" customFormat="1">
+      <c r="K49" s="48"/>
+    </row>
+    <row r="50" spans="11:11" s="21" customFormat="1">
+      <c r="K50" s="48"/>
+    </row>
+    <row r="51" spans="11:11" s="21" customFormat="1">
+      <c r="K51" s="48"/>
+    </row>
+    <row r="52" spans="11:11" s="21" customFormat="1">
+      <c r="K52" s="48"/>
+    </row>
+    <row r="53" spans="11:11" s="21" customFormat="1">
+      <c r="K53" s="48"/>
+    </row>
+    <row r="54" spans="11:11" s="21" customFormat="1">
+      <c r="K54" s="48"/>
+    </row>
+    <row r="55" spans="11:11" s="21" customFormat="1">
+      <c r="K55" s="48"/>
+    </row>
+    <row r="56" spans="11:11" s="21" customFormat="1">
+      <c r="K56" s="48"/>
+    </row>
+    <row r="57" spans="11:11" s="21" customFormat="1">
+      <c r="K57" s="48"/>
+    </row>
+    <row r="58" spans="11:11" s="21" customFormat="1">
+      <c r="K58" s="48"/>
+    </row>
+    <row r="59" spans="11:11" s="21" customFormat="1">
+      <c r="K59" s="48"/>
+    </row>
+    <row r="60" spans="11:11" s="21" customFormat="1">
+      <c r="K60" s="48"/>
+    </row>
+    <row r="61" spans="11:11" s="21" customFormat="1">
+      <c r="K61" s="48"/>
+    </row>
+    <row r="62" spans="11:11" s="21" customFormat="1">
+      <c r="K62" s="48"/>
+    </row>
+    <row r="63" spans="11:11" s="21" customFormat="1">
+      <c r="K63" s="48"/>
+    </row>
+    <row r="64" spans="11:11" s="21" customFormat="1">
+      <c r="K64" s="48"/>
+    </row>
+    <row r="65" spans="11:11" s="21" customFormat="1">
+      <c r="K65" s="48"/>
+    </row>
+    <row r="66" spans="11:11" s="21" customFormat="1">
+      <c r="K66" s="48"/>
+    </row>
+    <row r="67" spans="11:11" s="21" customFormat="1">
+      <c r="K67" s="48"/>
+    </row>
+    <row r="68" spans="11:11" s="21" customFormat="1">
+      <c r="K68" s="48"/>
+    </row>
+    <row r="69" spans="11:11" s="21" customFormat="1">
+      <c r="K69" s="48"/>
+    </row>
+    <row r="70" spans="11:11" s="21" customFormat="1">
+      <c r="K70" s="48"/>
+    </row>
+    <row r="71" spans="11:11" s="21" customFormat="1">
+      <c r="K71" s="48"/>
+    </row>
+    <row r="72" spans="11:11" s="21" customFormat="1">
+      <c r="K72" s="48"/>
+    </row>
+    <row r="73" spans="11:11" s="21" customFormat="1">
+      <c r="K73" s="48"/>
+    </row>
+    <row r="74" spans="11:11" s="21" customFormat="1">
+      <c r="K74" s="48"/>
+    </row>
+    <row r="75" spans="11:11" s="21" customFormat="1">
+      <c r="K75" s="48"/>
+    </row>
+    <row r="76" spans="11:11" s="21" customFormat="1">
+      <c r="K76" s="48"/>
+    </row>
+    <row r="77" spans="11:11" s="21" customFormat="1">
+      <c r="K77" s="48"/>
+    </row>
+    <row r="78" spans="11:11" s="21" customFormat="1">
+      <c r="K78" s="48"/>
+    </row>
+    <row r="79" spans="11:11" s="21" customFormat="1">
+      <c r="K79" s="48"/>
+    </row>
+    <row r="80" spans="11:11" s="21" customFormat="1">
+      <c r="K80" s="48"/>
+    </row>
+    <row r="81" spans="11:11" s="21" customFormat="1">
+      <c r="K81" s="48"/>
+    </row>
+    <row r="82" spans="11:11" s="21" customFormat="1">
+      <c r="K82" s="48"/>
+    </row>
+    <row r="83" spans="11:11" s="21" customFormat="1">
+      <c r="K83" s="48"/>
+    </row>
+    <row r="84" spans="11:11" s="21" customFormat="1">
+      <c r="K84" s="48"/>
+    </row>
+    <row r="85" spans="11:11" s="21" customFormat="1">
+      <c r="K85" s="48"/>
+    </row>
+    <row r="86" spans="11:11" s="21" customFormat="1">
+      <c r="K86" s="48"/>
+    </row>
+    <row r="87" spans="11:11" s="21" customFormat="1">
+      <c r="K87" s="48"/>
+    </row>
+    <row r="88" spans="11:11" s="21" customFormat="1">
+      <c r="K88" s="48"/>
+    </row>
+    <row r="89" spans="11:11" s="21" customFormat="1">
+      <c r="K89" s="48"/>
+    </row>
+    <row r="90" spans="11:11" s="21" customFormat="1">
+      <c r="K90" s="48"/>
+    </row>
+    <row r="91" spans="11:11" s="21" customFormat="1">
+      <c r="K91" s="48"/>
+    </row>
+    <row r="92" spans="11:11" s="21" customFormat="1">
+      <c r="K92" s="48"/>
+    </row>
+    <row r="93" spans="11:11" s="21" customFormat="1">
+      <c r="K93" s="48"/>
+    </row>
+    <row r="94" spans="11:11" s="21" customFormat="1">
+      <c r="K94" s="48"/>
+    </row>
+    <row r="95" spans="11:11" s="21" customFormat="1">
+      <c r="K95" s="48"/>
+    </row>
+    <row r="96" spans="11:11" s="21" customFormat="1">
+      <c r="K96" s="48"/>
+    </row>
+    <row r="97" spans="11:11" s="21" customFormat="1">
+      <c r="K97" s="48"/>
+    </row>
+    <row r="98" spans="11:11" s="21" customFormat="1">
+      <c r="K98" s="48"/>
+    </row>
+    <row r="99" spans="11:11" s="21" customFormat="1">
+      <c r="K99" s="48"/>
+    </row>
+    <row r="100" spans="11:11" s="21" customFormat="1">
+      <c r="K100" s="48"/>
+    </row>
+    <row r="101" spans="11:11" s="21" customFormat="1">
+      <c r="K101" s="48"/>
+    </row>
+    <row r="102" spans="11:11" s="21" customFormat="1">
+      <c r="K102" s="48"/>
+    </row>
+    <row r="103" spans="11:11" s="21" customFormat="1">
+      <c r="K103" s="48"/>
+    </row>
+    <row r="104" spans="11:11" s="21" customFormat="1">
+      <c r="K104" s="48"/>
+    </row>
+    <row r="105" spans="11:11" s="21" customFormat="1">
+      <c r="K105" s="48"/>
+    </row>
+    <row r="106" spans="11:11" s="21" customFormat="1">
+      <c r="K106" s="48"/>
+    </row>
+    <row r="107" spans="11:11" s="21" customFormat="1">
+      <c r="K107" s="48"/>
+    </row>
+    <row r="108" spans="11:11" s="21" customFormat="1">
+      <c r="K108" s="48"/>
+    </row>
+    <row r="109" spans="11:11" s="21" customFormat="1">
+      <c r="K109" s="48"/>
+    </row>
+    <row r="110" spans="11:11" s="21" customFormat="1">
+      <c r="K110" s="48"/>
+    </row>
+    <row r="111" spans="11:11" s="21" customFormat="1">
+      <c r="K111" s="48"/>
+    </row>
+    <row r="112" spans="11:11" s="21" customFormat="1">
+      <c r="K112" s="48"/>
+    </row>
+    <row r="113" spans="11:11" s="21" customFormat="1">
+      <c r="K113" s="48"/>
+    </row>
+    <row r="114" spans="11:11" s="21" customFormat="1">
+      <c r="K114" s="48"/>
+    </row>
+    <row r="115" spans="11:11" s="21" customFormat="1">
+      <c r="K115" s="48"/>
+    </row>
+    <row r="116" spans="11:11" s="21" customFormat="1">
+      <c r="K116" s="48"/>
+    </row>
+    <row r="117" spans="11:11" s="21" customFormat="1">
+      <c r="K117" s="48"/>
+    </row>
+    <row r="118" spans="11:11" s="21" customFormat="1">
+      <c r="K118" s="48"/>
+    </row>
+    <row r="119" spans="11:11" s="21" customFormat="1">
+      <c r="K119" s="48"/>
+    </row>
+    <row r="120" spans="11:11" s="21" customFormat="1">
+      <c r="K120" s="48"/>
+    </row>
+    <row r="121" spans="11:11" s="21" customFormat="1">
+      <c r="K121" s="48"/>
+    </row>
+    <row r="122" spans="11:11" s="21" customFormat="1">
+      <c r="K122" s="48"/>
+    </row>
+    <row r="123" spans="11:11" s="21" customFormat="1">
+      <c r="K123" s="48"/>
+    </row>
+    <row r="124" spans="11:11" s="21" customFormat="1">
+      <c r="K124" s="48"/>
+    </row>
+    <row r="125" spans="11:11" s="21" customFormat="1">
+      <c r="K125" s="48"/>
+    </row>
+    <row r="126" spans="11:11" s="21" customFormat="1">
+      <c r="K126" s="48"/>
+    </row>
+    <row r="127" spans="11:11" s="21" customFormat="1">
+      <c r="K127" s="48"/>
+    </row>
+    <row r="128" spans="11:11" s="21" customFormat="1">
+      <c r="K128" s="48"/>
+    </row>
+    <row r="129" spans="11:11" s="21" customFormat="1">
+      <c r="K129" s="48"/>
+    </row>
+    <row r="130" spans="11:11" s="21" customFormat="1">
+      <c r="K130" s="48"/>
+    </row>
+    <row r="131" spans="11:11" s="21" customFormat="1">
+      <c r="K131" s="48"/>
+    </row>
+    <row r="132" spans="11:11" s="21" customFormat="1">
+      <c r="K132" s="48"/>
+    </row>
+    <row r="133" spans="11:11" s="21" customFormat="1">
+      <c r="K133" s="48"/>
+    </row>
+    <row r="134" spans="11:11" s="21" customFormat="1">
+      <c r="K134" s="48"/>
+    </row>
+    <row r="135" spans="11:11" s="21" customFormat="1">
+      <c r="K135" s="48"/>
+    </row>
+    <row r="136" spans="11:11" s="21" customFormat="1">
+      <c r="K136" s="48"/>
+    </row>
+    <row r="137" spans="11:11" s="21" customFormat="1">
+      <c r="K137" s="48"/>
+    </row>
+    <row r="138" spans="11:11" s="21" customFormat="1">
+      <c r="K138" s="48"/>
+    </row>
+    <row r="139" spans="11:11" s="21" customFormat="1">
+      <c r="K139" s="48"/>
+    </row>
+    <row r="140" spans="11:11" s="21" customFormat="1">
+      <c r="K140" s="48"/>
+    </row>
+    <row r="141" spans="11:11" s="21" customFormat="1">
+      <c r="K141" s="48"/>
+    </row>
+    <row r="142" spans="11:11" s="21" customFormat="1">
+      <c r="K142" s="48"/>
+    </row>
+    <row r="143" spans="11:11" s="21" customFormat="1">
+      <c r="K143" s="48"/>
+    </row>
+    <row r="144" spans="11:11" s="21" customFormat="1">
+      <c r="K144" s="48"/>
+    </row>
+    <row r="145" spans="11:11" s="21" customFormat="1">
+      <c r="K145" s="48"/>
+    </row>
+    <row r="146" spans="11:11" s="21" customFormat="1">
+      <c r="K146" s="48"/>
+    </row>
+    <row r="147" spans="11:11" s="21" customFormat="1">
+      <c r="K147" s="48"/>
+    </row>
+    <row r="148" spans="11:11" s="21" customFormat="1">
+      <c r="K148" s="48"/>
+    </row>
+    <row r="149" spans="11:11" s="21" customFormat="1">
+      <c r="K149" s="48"/>
+    </row>
+    <row r="150" spans="11:11" s="21" customFormat="1">
+      <c r="K150" s="48"/>
+    </row>
+    <row r="151" spans="11:11" s="21" customFormat="1">
+      <c r="K151" s="48"/>
+    </row>
+    <row r="152" spans="11:11" s="21" customFormat="1">
+      <c r="K152" s="48"/>
+    </row>
+    <row r="153" spans="11:11" s="21" customFormat="1">
+      <c r="K153" s="48"/>
+    </row>
+    <row r="154" spans="11:11" s="21" customFormat="1">
+      <c r="K154" s="48"/>
+    </row>
+    <row r="155" spans="11:11" s="21" customFormat="1">
+      <c r="K155" s="48"/>
+    </row>
+    <row r="156" spans="11:11" s="21" customFormat="1">
+      <c r="K156" s="48"/>
+    </row>
+    <row r="157" spans="11:11" s="21" customFormat="1">
+      <c r="K157" s="48"/>
+    </row>
+    <row r="158" spans="11:11" s="21" customFormat="1">
+      <c r="K158" s="48"/>
+    </row>
+    <row r="159" spans="11:11" s="21" customFormat="1">
+      <c r="K159" s="48"/>
+    </row>
+    <row r="160" spans="11:11" s="21" customFormat="1">
+      <c r="K160" s="48"/>
+    </row>
+    <row r="161" spans="11:11" s="21" customFormat="1">
+      <c r="K161" s="48"/>
+    </row>
+    <row r="162" spans="11:11" s="21" customFormat="1">
+      <c r="K162" s="48"/>
+    </row>
+    <row r="163" spans="11:11" s="21" customFormat="1">
+      <c r="K163" s="48"/>
+    </row>
+    <row r="164" spans="11:11" s="21" customFormat="1">
+      <c r="K164" s="48"/>
+    </row>
+    <row r="165" spans="11:11" s="21" customFormat="1">
+      <c r="K165" s="48"/>
+    </row>
+    <row r="166" spans="11:11" s="21" customFormat="1">
+      <c r="K166" s="48"/>
+    </row>
+    <row r="167" spans="11:11" s="21" customFormat="1">
+      <c r="K167" s="48"/>
+    </row>
+    <row r="168" spans="11:11" s="21" customFormat="1">
+      <c r="K168" s="48"/>
+    </row>
+    <row r="169" spans="11:11" s="21" customFormat="1">
+      <c r="K169" s="48"/>
+    </row>
+    <row r="170" spans="11:11" s="21" customFormat="1">
+      <c r="K170" s="48"/>
+    </row>
+    <row r="171" spans="11:11" s="21" customFormat="1">
+      <c r="K171" s="48"/>
+    </row>
+    <row r="172" spans="11:11" s="21" customFormat="1">
+      <c r="K172" s="48"/>
+    </row>
+    <row r="173" spans="11:11" s="21" customFormat="1">
+      <c r="K173" s="48"/>
+    </row>
+    <row r="174" spans="11:11" s="21" customFormat="1">
+      <c r="K174" s="48"/>
+    </row>
+    <row r="175" spans="11:11" s="21" customFormat="1">
+      <c r="K175" s="48"/>
+    </row>
+    <row r="176" spans="11:11" s="21" customFormat="1">
+      <c r="K176" s="48"/>
+    </row>
+    <row r="177" spans="11:11" s="21" customFormat="1">
+      <c r="K177" s="48"/>
+    </row>
+    <row r="178" spans="11:11" s="21" customFormat="1">
+      <c r="K178" s="48"/>
+    </row>
+    <row r="179" spans="11:11" s="21" customFormat="1">
+      <c r="K179" s="48"/>
+    </row>
+    <row r="180" spans="11:11" s="21" customFormat="1">
+      <c r="K180" s="48"/>
+    </row>
+    <row r="181" spans="11:11" s="21" customFormat="1">
+      <c r="K181" s="48"/>
+    </row>
+    <row r="182" spans="11:11" s="21" customFormat="1">
+      <c r="K182" s="48"/>
+    </row>
+    <row r="183" spans="11:11" s="21" customFormat="1">
+      <c r="K183" s="48"/>
+    </row>
+    <row r="184" spans="11:11" s="21" customFormat="1">
+      <c r="K184" s="48"/>
+    </row>
+    <row r="185" spans="11:11" s="21" customFormat="1">
+      <c r="K185" s="48"/>
+    </row>
+    <row r="186" spans="11:11" s="21" customFormat="1">
+      <c r="K186" s="48"/>
+    </row>
+    <row r="187" spans="11:11" s="21" customFormat="1">
+      <c r="K187" s="48"/>
+    </row>
+    <row r="188" spans="11:11" s="21" customFormat="1">
+      <c r="K188" s="48"/>
+    </row>
+    <row r="189" spans="11:11" s="21" customFormat="1">
+      <c r="K189" s="48"/>
+    </row>
+    <row r="190" spans="11:11" s="21" customFormat="1">
+      <c r="K190" s="48"/>
+    </row>
+    <row r="191" spans="11:11" s="21" customFormat="1">
+      <c r="K191" s="48"/>
+    </row>
+    <row r="192" spans="11:11" s="21" customFormat="1">
+      <c r="K192" s="48"/>
+    </row>
+    <row r="193" spans="11:11" s="21" customFormat="1">
+      <c r="K193" s="48"/>
+    </row>
+    <row r="194" spans="11:11" s="21" customFormat="1">
+      <c r="K194" s="48"/>
+    </row>
+    <row r="195" spans="11:11" s="21" customFormat="1">
+      <c r="K195" s="48"/>
+    </row>
+    <row r="196" spans="11:11" s="21" customFormat="1">
+      <c r="K196" s="48"/>
+    </row>
+    <row r="197" spans="11:11" s="21" customFormat="1">
+      <c r="K197" s="48"/>
+    </row>
+    <row r="198" spans="11:11" s="21" customFormat="1">
+      <c r="K198" s="48"/>
+    </row>
+    <row r="199" spans="11:11" s="21" customFormat="1">
+      <c r="K199" s="48"/>
+    </row>
+    <row r="200" spans="11:11" s="21" customFormat="1">
+      <c r="K200" s="48"/>
+    </row>
+    <row r="201" spans="11:11" s="21" customFormat="1">
+      <c r="K201" s="48"/>
+    </row>
+    <row r="202" spans="11:11" s="21" customFormat="1">
+      <c r="K202" s="48"/>
+    </row>
+    <row r="203" spans="11:11" s="21" customFormat="1">
+      <c r="K203" s="48"/>
+    </row>
+    <row r="204" spans="11:11" s="21" customFormat="1">
+      <c r="K204" s="48"/>
+    </row>
+    <row r="205" spans="11:11" s="21" customFormat="1">
+      <c r="K205" s="48"/>
+    </row>
+    <row r="206" spans="11:11" s="21" customFormat="1">
+      <c r="K206" s="48"/>
+    </row>
+    <row r="207" spans="11:11" s="21" customFormat="1">
+      <c r="K207" s="48"/>
+    </row>
+    <row r="208" spans="11:11" s="21" customFormat="1">
+      <c r="K208" s="48"/>
+    </row>
+    <row r="209" spans="11:11" s="21" customFormat="1">
+      <c r="K209" s="48"/>
+    </row>
+    <row r="210" spans="11:11" s="21" customFormat="1">
+      <c r="K210" s="48"/>
+    </row>
+    <row r="211" spans="11:11" s="21" customFormat="1">
+      <c r="K211" s="48"/>
+    </row>
+    <row r="212" spans="11:11" s="21" customFormat="1">
+      <c r="K212" s="48"/>
+    </row>
+    <row r="213" spans="11:11" s="21" customFormat="1">
+      <c r="K213" s="48"/>
+    </row>
+    <row r="214" spans="11:11" s="21" customFormat="1">
+      <c r="K214" s="48"/>
+    </row>
+    <row r="215" spans="11:11" s="21" customFormat="1">
+      <c r="K215" s="48"/>
+    </row>
+    <row r="216" spans="11:11" s="21" customFormat="1">
+      <c r="K216" s="48"/>
+    </row>
+    <row r="217" spans="11:11" s="21" customFormat="1">
+      <c r="K217" s="48"/>
+    </row>
+    <row r="218" spans="11:11" s="21" customFormat="1">
+      <c r="K218" s="48"/>
+    </row>
+    <row r="219" spans="11:11" s="21" customFormat="1">
+      <c r="K219" s="48"/>
+    </row>
+    <row r="220" spans="11:11" s="21" customFormat="1">
+      <c r="K220" s="48"/>
+    </row>
+    <row r="221" spans="11:11" s="21" customFormat="1">
+      <c r="K221" s="48"/>
+    </row>
+    <row r="222" spans="11:11" s="21" customFormat="1">
+      <c r="K222" s="48"/>
+    </row>
+    <row r="223" spans="11:11" s="21" customFormat="1">
+      <c r="K223" s="48"/>
+    </row>
+    <row r="224" spans="11:11" s="21" customFormat="1">
+      <c r="K224" s="48"/>
+    </row>
+    <row r="225" spans="11:11" s="21" customFormat="1">
+      <c r="K225" s="48"/>
+    </row>
+    <row r="226" spans="11:11" s="21" customFormat="1">
+      <c r="K226" s="48"/>
+    </row>
+    <row r="227" spans="11:11" s="21" customFormat="1">
+      <c r="K227" s="48"/>
+    </row>
+    <row r="228" spans="11:11" s="21" customFormat="1">
+      <c r="K228" s="48"/>
+    </row>
+    <row r="229" spans="11:11" s="21" customFormat="1">
+      <c r="K229" s="48"/>
+    </row>
+    <row r="230" spans="11:11" s="21" customFormat="1">
+      <c r="K230" s="48"/>
+    </row>
+    <row r="231" spans="11:11" s="21" customFormat="1">
+      <c r="K231" s="48"/>
+    </row>
+    <row r="232" spans="11:11" s="21" customFormat="1">
+      <c r="K232" s="48"/>
+    </row>
+    <row r="233" spans="11:11" s="21" customFormat="1">
+      <c r="K233" s="48"/>
+    </row>
+    <row r="234" spans="11:11" s="21" customFormat="1">
+      <c r="K234" s="48"/>
+    </row>
+    <row r="235" spans="11:11" s="21" customFormat="1">
+      <c r="K235" s="48"/>
+    </row>
+    <row r="236" spans="11:11" s="21" customFormat="1">
+      <c r="K236" s="48"/>
+    </row>
+    <row r="237" spans="11:11" s="21" customFormat="1">
+      <c r="K237" s="48"/>
+    </row>
+    <row r="238" spans="11:11" s="21" customFormat="1">
+      <c r="K238" s="48"/>
+    </row>
+    <row r="239" spans="11:11" s="21" customFormat="1">
+      <c r="K239" s="48"/>
+    </row>
+    <row r="240" spans="11:11" s="21" customFormat="1">
+      <c r="K240" s="48"/>
+    </row>
+    <row r="241" spans="11:11" s="21" customFormat="1">
+      <c r="K241" s="48"/>
+    </row>
+    <row r="242" spans="11:11" s="21" customFormat="1">
+      <c r="K242" s="48"/>
+    </row>
+    <row r="243" spans="11:11" s="21" customFormat="1">
+      <c r="K243" s="48"/>
+    </row>
+    <row r="244" spans="11:11" s="21" customFormat="1">
+      <c r="K244" s="48"/>
+    </row>
+    <row r="245" spans="11:11" s="21" customFormat="1">
+      <c r="K245" s="48"/>
+    </row>
+    <row r="246" spans="11:11" s="21" customFormat="1">
+      <c r="K246" s="48"/>
+    </row>
+    <row r="247" spans="11:11" s="21" customFormat="1">
+      <c r="K247" s="48"/>
+    </row>
+    <row r="248" spans="11:11" s="21" customFormat="1">
+      <c r="K248" s="48"/>
+    </row>
+    <row r="249" spans="11:11" s="21" customFormat="1">
+      <c r="K249" s="48"/>
+    </row>
+    <row r="250" spans="11:11" s="21" customFormat="1">
+      <c r="K250" s="48"/>
+    </row>
+    <row r="251" spans="11:11" s="21" customFormat="1">
+      <c r="K251" s="48"/>
+    </row>
+    <row r="252" spans="11:11" s="21" customFormat="1">
+      <c r="K252" s="48"/>
+    </row>
+    <row r="253" spans="11:11" s="21" customFormat="1">
+      <c r="K253" s="48"/>
+    </row>
+    <row r="254" spans="11:11" s="21" customFormat="1">
+      <c r="K254" s="48"/>
+    </row>
+    <row r="255" spans="11:11" s="21" customFormat="1">
+      <c r="K255" s="48"/>
+    </row>
+    <row r="256" spans="11:11" s="21" customFormat="1">
+      <c r="K256" s="48"/>
+    </row>
+    <row r="257" spans="11:11" s="21" customFormat="1">
+      <c r="K257" s="48"/>
+    </row>
+    <row r="258" spans="11:11" s="21" customFormat="1">
+      <c r="K258" s="48"/>
+    </row>
+    <row r="259" spans="11:11" s="21" customFormat="1">
+      <c r="K259" s="48"/>
+    </row>
+    <row r="260" spans="11:11" s="21" customFormat="1">
+      <c r="K260" s="48"/>
+    </row>
+    <row r="261" spans="11:11" s="21" customFormat="1">
+      <c r="K261" s="48"/>
+    </row>
+    <row r="262" spans="11:11" s="21" customFormat="1">
+      <c r="K262" s="48"/>
+    </row>
+    <row r="263" spans="11:11" s="21" customFormat="1">
+      <c r="K263" s="48"/>
+    </row>
+    <row r="264" spans="11:11" s="21" customFormat="1">
+      <c r="K264" s="48"/>
+    </row>
+    <row r="265" spans="11:11" s="21" customFormat="1">
+      <c r="K265" s="48"/>
+    </row>
+    <row r="266" spans="11:11" s="21" customFormat="1">
+      <c r="K266" s="48"/>
+    </row>
+    <row r="267" spans="11:11" s="21" customFormat="1">
+      <c r="K267" s="48"/>
+    </row>
+    <row r="268" spans="11:11" s="21" customFormat="1">
+      <c r="K268" s="48"/>
+    </row>
+    <row r="269" spans="11:11" s="21" customFormat="1">
+      <c r="K269" s="48"/>
+    </row>
+    <row r="270" spans="11:11" s="21" customFormat="1">
+      <c r="K270" s="48"/>
+    </row>
+    <row r="271" spans="11:11" s="21" customFormat="1">
+      <c r="K271" s="48"/>
+    </row>
+    <row r="272" spans="11:11" s="21" customFormat="1">
+      <c r="K272" s="48"/>
+    </row>
+    <row r="273" spans="11:11" s="21" customFormat="1">
+      <c r="K273" s="48"/>
+    </row>
+    <row r="274" spans="11:11" s="21" customFormat="1">
+      <c r="K274" s="48"/>
+    </row>
+    <row r="275" spans="11:11" s="21" customFormat="1">
+      <c r="K275" s="48"/>
+    </row>
+    <row r="276" spans="11:11" s="21" customFormat="1">
+      <c r="K276" s="48"/>
+    </row>
+    <row r="277" spans="11:11" s="21" customFormat="1">
+      <c r="K277" s="48"/>
+    </row>
+    <row r="278" spans="11:11" s="21" customFormat="1">
+      <c r="K278" s="48"/>
+    </row>
+    <row r="279" spans="11:11" s="21" customFormat="1">
+      <c r="K279" s="48"/>
+    </row>
+    <row r="280" spans="11:11" s="21" customFormat="1">
+      <c r="K280" s="48"/>
+    </row>
+    <row r="281" spans="11:11" s="21" customFormat="1">
+      <c r="K281" s="48"/>
+    </row>
+    <row r="282" spans="11:11" s="21" customFormat="1">
+      <c r="K282" s="48"/>
+    </row>
+    <row r="283" spans="11:11" s="21" customFormat="1">
+      <c r="K283" s="48"/>
+    </row>
+    <row r="284" spans="11:11" s="21" customFormat="1">
+      <c r="K284" s="48"/>
+    </row>
+    <row r="285" spans="11:11" s="21" customFormat="1">
+      <c r="K285" s="48"/>
+    </row>
+    <row r="286" spans="11:11" s="21" customFormat="1">
+      <c r="K286" s="48"/>
+    </row>
+    <row r="287" spans="11:11" s="21" customFormat="1">
+      <c r="K287" s="48"/>
+    </row>
+    <row r="288" spans="11:11" s="21" customFormat="1">
+      <c r="K288" s="48"/>
+    </row>
+    <row r="289" spans="11:11" s="21" customFormat="1">
+      <c r="K289" s="48"/>
+    </row>
+    <row r="290" spans="11:11" s="21" customFormat="1">
+      <c r="K290" s="48"/>
+    </row>
+    <row r="291" spans="11:11" s="21" customFormat="1">
+      <c r="K291" s="48"/>
+    </row>
+    <row r="292" spans="11:11" s="21" customFormat="1">
+      <c r="K292" s="48"/>
+    </row>
+    <row r="293" spans="11:11" s="21" customFormat="1">
+      <c r="K293" s="48"/>
+    </row>
+    <row r="294" spans="11:11" s="21" customFormat="1">
+      <c r="K294" s="48"/>
+    </row>
+    <row r="295" spans="11:11" s="21" customFormat="1">
+      <c r="K295" s="48"/>
+    </row>
+    <row r="296" spans="11:11" s="21" customFormat="1">
+      <c r="K296" s="48"/>
+    </row>
+    <row r="297" spans="11:11" s="21" customFormat="1">
+      <c r="K297" s="48"/>
+    </row>
+    <row r="298" spans="11:11" s="21" customFormat="1">
+      <c r="K298" s="48"/>
+    </row>
+    <row r="299" spans="11:11" s="21" customFormat="1">
+      <c r="K299" s="48"/>
+    </row>
+    <row r="300" spans="11:11" s="21" customFormat="1">
+      <c r="K300" s="48"/>
+    </row>
+    <row r="301" spans="11:11" s="21" customFormat="1">
+      <c r="K301" s="48"/>
+    </row>
+    <row r="302" spans="11:11" s="21" customFormat="1">
+      <c r="K302" s="48"/>
+    </row>
+    <row r="303" spans="11:11" s="21" customFormat="1">
+      <c r="K303" s="48"/>
+    </row>
+    <row r="304" spans="11:11" s="21" customFormat="1">
+      <c r="K304" s="48"/>
+    </row>
+    <row r="305" spans="11:11" s="21" customFormat="1">
+      <c r="K305" s="48"/>
+    </row>
+    <row r="306" spans="11:11" s="21" customFormat="1">
+      <c r="K306" s="48"/>
+    </row>
+    <row r="307" spans="11:11" s="21" customFormat="1">
+      <c r="K307" s="48"/>
+    </row>
+    <row r="308" spans="11:11" s="21" customFormat="1">
+      <c r="K308" s="48"/>
+    </row>
+    <row r="309" spans="11:11" s="21" customFormat="1">
+      <c r="K309" s="48"/>
+    </row>
+    <row r="310" spans="11:11" s="21" customFormat="1">
+      <c r="K310" s="48"/>
+    </row>
+    <row r="311" spans="11:11" s="21" customFormat="1">
+      <c r="K311" s="48"/>
+    </row>
+    <row r="312" spans="11:11" s="21" customFormat="1">
+      <c r="K312" s="48"/>
+    </row>
+    <row r="313" spans="11:11" s="21" customFormat="1">
+      <c r="K313" s="48"/>
+    </row>
+    <row r="314" spans="11:11" s="21" customFormat="1">
+      <c r="K314" s="48"/>
+    </row>
+    <row r="315" spans="11:11" s="21" customFormat="1">
+      <c r="K315" s="48"/>
+    </row>
+    <row r="316" spans="11:11" s="21" customFormat="1">
+      <c r="K316" s="48"/>
+    </row>
+    <row r="317" spans="11:11" s="21" customFormat="1">
+      <c r="K317" s="48"/>
+    </row>
+    <row r="318" spans="11:11" s="21" customFormat="1">
+      <c r="K318" s="48"/>
+    </row>
+    <row r="319" spans="11:11" s="21" customFormat="1">
+      <c r="K319" s="48"/>
+    </row>
+    <row r="320" spans="11:11" s="21" customFormat="1">
+      <c r="K320" s="48"/>
+    </row>
+    <row r="321" spans="11:11" s="21" customFormat="1">
+      <c r="K321" s="48"/>
+    </row>
+    <row r="322" spans="11:11" s="21" customFormat="1">
+      <c r="K322" s="48"/>
+    </row>
+    <row r="323" spans="11:11" s="21" customFormat="1">
+      <c r="K323" s="48"/>
+    </row>
+    <row r="324" spans="11:11" s="21" customFormat="1">
+      <c r="K324" s="48"/>
+    </row>
+    <row r="325" spans="11:11" s="21" customFormat="1">
+      <c r="K325" s="48"/>
+    </row>
+    <row r="326" spans="11:11" s="21" customFormat="1">
+      <c r="K326" s="48"/>
+    </row>
+    <row r="327" spans="11:11" s="21" customFormat="1">
+      <c r="K327" s="48"/>
+    </row>
+    <row r="328" spans="11:11" s="21" customFormat="1">
+      <c r="K328" s="48"/>
+    </row>
+    <row r="329" spans="11:11" s="21" customFormat="1">
+      <c r="K329" s="48"/>
+    </row>
+    <row r="330" spans="11:11" s="21" customFormat="1">
+      <c r="K330" s="48"/>
+    </row>
+    <row r="331" spans="11:11" s="21" customFormat="1">
+      <c r="K331" s="48"/>
+    </row>
+    <row r="332" spans="11:11" s="21" customFormat="1">
+      <c r="K332" s="48"/>
+    </row>
+    <row r="333" spans="11:11" s="21" customFormat="1">
+      <c r="K333" s="48"/>
+    </row>
+    <row r="334" spans="11:11" s="21" customFormat="1">
+      <c r="K334" s="48"/>
+    </row>
+    <row r="335" spans="11:11" s="21" customFormat="1">
+      <c r="K335" s="48"/>
+    </row>
+    <row r="336" spans="11:11" s="21" customFormat="1">
+      <c r="K336" s="48"/>
+    </row>
+    <row r="337" spans="11:11" s="21" customFormat="1">
+      <c r="K337" s="48"/>
+    </row>
+    <row r="338" spans="11:11" s="21" customFormat="1">
+      <c r="K338" s="48"/>
+    </row>
+    <row r="339" spans="11:11" s="21" customFormat="1">
+      <c r="K339" s="48"/>
+    </row>
+    <row r="340" spans="11:11" s="21" customFormat="1">
+      <c r="K340" s="48"/>
+    </row>
+    <row r="341" spans="11:11" s="21" customFormat="1">
+      <c r="K341" s="48"/>
+    </row>
+    <row r="342" spans="11:11" s="21" customFormat="1">
+      <c r="K342" s="48"/>
+    </row>
+    <row r="343" spans="11:11" s="21" customFormat="1">
+      <c r="K343" s="48"/>
+    </row>
+    <row r="344" spans="11:11" s="21" customFormat="1">
+      <c r="K344" s="48"/>
+    </row>
+    <row r="345" spans="11:11" s="21" customFormat="1">
+      <c r="K345" s="48"/>
+    </row>
+    <row r="346" spans="11:11" s="21" customFormat="1">
+      <c r="K346" s="48"/>
+    </row>
+    <row r="347" spans="11:11" s="21" customFormat="1">
+      <c r="K347" s="48"/>
+    </row>
+    <row r="348" spans="11:11" s="21" customFormat="1">
+      <c r="K348" s="48"/>
+    </row>
+    <row r="349" spans="11:11" s="21" customFormat="1">
+      <c r="K349" s="48"/>
+    </row>
+    <row r="350" spans="11:11" s="21" customFormat="1">
+      <c r="K350" s="48"/>
+    </row>
+    <row r="351" spans="11:11" s="21" customFormat="1">
+      <c r="K351" s="48"/>
+    </row>
+    <row r="352" spans="11:11" s="21" customFormat="1">
+      <c r="K352" s="48"/>
+    </row>
+    <row r="353" spans="11:11" s="21" customFormat="1">
+      <c r="K353" s="48"/>
+    </row>
+    <row r="354" spans="11:11" s="21" customFormat="1">
+      <c r="K354" s="48"/>
+    </row>
+    <row r="355" spans="11:11" s="21" customFormat="1">
+      <c r="K355" s="48"/>
+    </row>
+    <row r="356" spans="11:11" s="21" customFormat="1">
+      <c r="K356" s="48"/>
+    </row>
+    <row r="357" spans="11:11" s="21" customFormat="1">
+      <c r="K357" s="48"/>
+    </row>
+    <row r="358" spans="11:11" s="21" customFormat="1">
+      <c r="K358" s="48"/>
+    </row>
+    <row r="359" spans="11:11" s="21" customFormat="1">
+      <c r="K359" s="48"/>
+    </row>
+    <row r="360" spans="11:11" s="21" customFormat="1">
+      <c r="K360" s="48"/>
+    </row>
+    <row r="361" spans="11:11" s="21" customFormat="1">
+      <c r="K361" s="48"/>
+    </row>
+    <row r="362" spans="11:11" s="21" customFormat="1">
+      <c r="K362" s="48"/>
+    </row>
+    <row r="363" spans="11:11" s="21" customFormat="1">
+      <c r="K363" s="48"/>
+    </row>
+    <row r="364" spans="11:11" s="21" customFormat="1">
+      <c r="K364" s="48"/>
+    </row>
+    <row r="365" spans="11:11" s="21" customFormat="1">
+      <c r="K365" s="48"/>
+    </row>
+    <row r="366" spans="11:11" s="21" customFormat="1">
+      <c r="K366" s="48"/>
+    </row>
+    <row r="367" spans="11:11" s="21" customFormat="1">
+      <c r="K367" s="48"/>
+    </row>
+    <row r="368" spans="11:11" s="21" customFormat="1">
+      <c r="K368" s="48"/>
+    </row>
+    <row r="369" spans="11:11" s="21" customFormat="1">
+      <c r="K369" s="48"/>
+    </row>
+    <row r="370" spans="11:11" s="21" customFormat="1">
+      <c r="K370" s="48"/>
+    </row>
+    <row r="371" spans="11:11" s="21" customFormat="1">
+      <c r="K371" s="48"/>
+    </row>
+    <row r="372" spans="11:11" s="21" customFormat="1">
+      <c r="K372" s="48"/>
+    </row>
+    <row r="373" spans="11:11" s="21" customFormat="1">
+      <c r="K373" s="48"/>
+    </row>
+    <row r="374" spans="11:11" s="21" customFormat="1">
+      <c r="K374" s="48"/>
+    </row>
+    <row r="375" spans="11:11" s="21" customFormat="1">
+      <c r="K375" s="48"/>
+    </row>
+    <row r="376" spans="11:11" s="21" customFormat="1">
+      <c r="K376" s="48"/>
+    </row>
+    <row r="377" spans="11:11" s="21" customFormat="1">
+      <c r="K377" s="48"/>
+    </row>
+    <row r="378" spans="11:11" s="21" customFormat="1">
+      <c r="K378" s="48"/>
+    </row>
+    <row r="379" spans="11:11" s="21" customFormat="1">
+      <c r="K379" s="48"/>
+    </row>
+    <row r="380" spans="11:11" s="21" customFormat="1">
+      <c r="K380" s="48"/>
+    </row>
+    <row r="381" spans="11:11" s="21" customFormat="1">
+      <c r="K381" s="48"/>
+    </row>
+    <row r="382" spans="11:11" s="21" customFormat="1">
+      <c r="K382" s="48"/>
+    </row>
+    <row r="383" spans="11:11" s="21" customFormat="1">
+      <c r="K383" s="48"/>
+    </row>
+    <row r="384" spans="11:11" s="21" customFormat="1">
+      <c r="K384" s="48"/>
+    </row>
+    <row r="385" spans="1:11" s="21" customFormat="1">
+      <c r="A385" s="1"/>
+      <c r="K385" s="48"/>
+    </row>
+    <row r="386" spans="1:11" s="21" customFormat="1">
+      <c r="A386" s="1"/>
+      <c r="K386" s="48"/>
+    </row>
+    <row r="387" spans="1:11" s="21" customFormat="1">
+      <c r="A387" s="1"/>
+      <c r="K387" s="48"/>
+    </row>
+    <row r="388" spans="1:11" s="21" customFormat="1">
+      <c r="A388" s="1"/>
+      <c r="K388" s="48"/>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:I58">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:J58">
       <formula1>"passed,failed,skipped,blocked"</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="A3" location="RTM!B7" tooltip="Landing Page" display="SC_OH_1"/>
+    <hyperlink ref="A4" location="RTM!B8" tooltip="Login Scenario" display="SC_OH_2"/>
+    <hyperlink ref="A5" location="RTM!B8" tooltip="Login Scenario" display="SC_OH_2"/>
+    <hyperlink ref="A6" location="RTM!B8" tooltip="Login Scenario" display="SC_OH_2"/>
+    <hyperlink ref="A7" location="RTM!B8" tooltip="Login Scenario" display="SC_OH_2"/>
+    <hyperlink ref="A8" location="RTM!B9" tooltip="Login Scenario" display="SC_OH_3"/>
+    <hyperlink ref="A9" location="RTM!B10" tooltip="Login Scenario" display="SC_OH_4"/>
+    <hyperlink ref="A10" location="RTM!B11" tooltip="Login Scenario" display="SC_OH_5"/>
+    <hyperlink ref="A11" location="RTM!B11" tooltip="Login Scenario" display="SC_OH_5"/>
+    <hyperlink ref="A12" location="RTM!B11" tooltip="Login Scenario" display="SC_OH_5"/>
+    <hyperlink ref="A13" location="RTM!B11" tooltip="Login Scenario" display="SC_OH_5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -1942,14 +3165,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.399999999999999" thickTop="1" thickBot="1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="40"/>
-      <c r="C1" s="40"/>
-      <c r="D1" s="40"/>
-      <c r="E1" s="40"/>
-      <c r="F1" s="41"/>
+      <c r="B1" s="41"/>
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="41"/>
+      <c r="F1" s="42"/>
     </row>
     <row r="2" spans="1:6" ht="13.9" thickTop="1" thickBot="1">
       <c r="A2" s="22"/>
@@ -2063,17 +3286,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Levels xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">L1</Levels>
-    <Category xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Module Artifact</Category>
-    <FolderName xmlns="952a6df7-b138-4f89-9bc4-e7a874ea3254" xsi:nil="true"/>
-    <Material_x0020_Type xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Extra Material</Material_x0020_Type>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010046351F880B96AE4B9BB4815879ADEBDD" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="487f15db4e05f84fdb19aa3f548b93b8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81372d4e-bcfc-4844-a57b-a09c5da71958" xmlns:ns3="952a6df7-b138-4f89-9bc4-e7a874ea3254" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="09419ac551552483846d59652a820d17" ns2:_="" ns3:_="">
     <xsd:import namespace="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
@@ -2243,11 +3455,18 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Levels xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">L1</Levels>
+    <Category xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Module Artifact</Category>
+    <FolderName xmlns="952a6df7-b138-4f89-9bc4-e7a874ea3254" xsi:nil="true"/>
+    <Material_x0020_Type xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Extra Material</Material_x0020_Type>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -2256,24 +3475,11 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{812CC0C1-FD42-47A7-BEBF-6413B223EE92}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="952a6df7-b138-4f89-9bc4-e7a874ea3254"/>
-    <ds:schemaRef ds:uri="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38E28044-843A-4D7D-9F1F-711CA3C23377}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2292,18 +3498,35 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{812CC0C1-FD42-47A7-BEBF-6413B223EE92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="952a6df7-b138-4f89-9bc4-e7a874ea3254"/>
+    <ds:schemaRef ds:uri="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E4DBA88-91AD-42CE-827B-50AA920D4CEA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67F96C4C-21BE-4526-9614-87D2A1A52CD5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E4DBA88-91AD-42CE-827B-50AA920D4CEA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
reset link scenario updated
</commit_message>
<xml_diff>
--- a/Test Template Document Corp.xlsx
+++ b/Test Template Document Corp.xlsx
@@ -936,37 +936,37 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="4" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="16" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1009,7 +1009,7 @@
         <xdr:cNvPr id="2154" name="Picture 2" descr="pcs">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006A080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006A080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1440,11 +1440,11 @@
   </cols>
   <sheetData>
     <row r="4" spans="2:4" s="4" customFormat="1" ht="22.5">
-      <c r="B4" s="44" t="s">
+      <c r="B4" s="49" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="44"/>
-      <c r="D4" s="44"/>
+      <c r="C4" s="49"/>
+      <c r="D4" s="49"/>
     </row>
     <row r="5" spans="2:4" s="5" customFormat="1" ht="15">
       <c r="C5" s="6"/>
@@ -1453,28 +1453,28 @@
       <c r="B7" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="45" t="s">
+      <c r="C7" s="50" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="46"/>
+      <c r="D7" s="51"/>
     </row>
     <row r="8" spans="2:4" ht="17.25" customHeight="1">
       <c r="B8" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="45" t="s">
+      <c r="C8" s="50" t="s">
         <v>36</v>
       </c>
-      <c r="D8" s="46"/>
+      <c r="D8" s="51"/>
     </row>
     <row r="9" spans="2:4" ht="31.5" customHeight="1">
       <c r="B9" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="47" t="s">
+      <c r="C9" s="52" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="48"/>
+      <c r="D9" s="53"/>
     </row>
     <row r="10" spans="2:4" ht="17.25" customHeight="1">
       <c r="B10" s="9"/>
@@ -1767,8 +1767,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M387"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36" defaultRowHeight="12.75"/>
@@ -3302,110 +3302,110 @@
   </cols>
   <sheetData>
     <row r="6" spans="3:6" ht="27.4">
-      <c r="C6" s="52" t="s">
+      <c r="C6" s="44" t="s">
         <v>134</v>
       </c>
-      <c r="D6" s="52"/>
-      <c r="E6" s="52"/>
-      <c r="F6" s="52"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="44"/>
+      <c r="F6" s="44"/>
     </row>
     <row r="7" spans="3:6" ht="27.4">
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-      <c r="E7" s="52"/>
-      <c r="F7" s="52"/>
+      <c r="C7" s="44"/>
+      <c r="D7" s="44"/>
+      <c r="E7" s="44"/>
+      <c r="F7" s="44"/>
     </row>
     <row r="8" spans="3:6" ht="27.4">
-      <c r="C8" s="52"/>
-      <c r="D8" s="52"/>
-      <c r="E8" s="52"/>
-      <c r="F8" s="52"/>
+      <c r="C8" s="44"/>
+      <c r="D8" s="44"/>
+      <c r="E8" s="44"/>
+      <c r="F8" s="44"/>
     </row>
     <row r="9" spans="3:6" ht="27.4">
-      <c r="C9" s="52"/>
-      <c r="D9" s="52" t="s">
+      <c r="C9" s="44"/>
+      <c r="D9" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="E9" s="52" t="s">
+      <c r="E9" s="44" t="s">
         <v>136</v>
       </c>
-      <c r="F9" s="52" t="s">
+      <c r="F9" s="44" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="3:6" s="54" customFormat="1" ht="27.4">
-      <c r="C10" s="53"/>
-      <c r="D10" s="53" t="s">
+    <row r="10" spans="3:6" s="46" customFormat="1" ht="27.4">
+      <c r="C10" s="45"/>
+      <c r="D10" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="E10" s="53" t="s">
+      <c r="E10" s="45" t="s">
         <v>137</v>
       </c>
-      <c r="F10" s="53" t="s">
+      <c r="F10" s="45" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="11" spans="3:6" s="56" customFormat="1" ht="27.4">
-      <c r="C11" s="55"/>
-      <c r="D11" s="55"/>
-      <c r="E11" s="55"/>
-      <c r="F11" s="55"/>
-    </row>
-    <row r="12" spans="3:6" s="56" customFormat="1" ht="27.4">
-      <c r="C12" s="55"/>
-      <c r="D12" s="57" t="s">
+    <row r="11" spans="3:6" s="48" customFormat="1" ht="27.4">
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+    </row>
+    <row r="12" spans="3:6" s="48" customFormat="1" ht="27.4">
+      <c r="C12" s="47"/>
+      <c r="D12" s="54" t="s">
         <v>140</v>
       </c>
-      <c r="E12" s="57"/>
-      <c r="F12" s="57"/>
+      <c r="E12" s="54"/>
+      <c r="F12" s="54"/>
     </row>
     <row r="13" spans="3:6" ht="27.4">
-      <c r="C13" s="52"/>
-      <c r="D13" s="52" t="s">
+      <c r="C13" s="44"/>
+      <c r="D13" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="E13" s="52" t="s">
+      <c r="E13" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="F13" s="52" t="s">
+      <c r="F13" s="44" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="14" spans="3:6" ht="27.4">
-      <c r="C14" s="52"/>
-      <c r="D14" s="52" t="s">
+      <c r="C14" s="44"/>
+      <c r="D14" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="E14" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="F14" s="52" t="s">
+      <c r="F14" s="44" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="15" spans="3:6" ht="27.4">
-      <c r="C15" s="52"/>
-      <c r="D15" s="52" t="s">
+      <c r="C15" s="44"/>
+      <c r="D15" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="E15" s="52" t="s">
+      <c r="E15" s="44" t="s">
         <v>138</v>
       </c>
-      <c r="F15" s="52" t="s">
+      <c r="F15" s="44" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="16" spans="3:6" ht="27.4">
-      <c r="C16" s="52"/>
-      <c r="D16" s="52"/>
-      <c r="E16" s="52"/>
-      <c r="F16" s="52"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
     </row>
     <row r="17" spans="3:6" ht="27.4">
-      <c r="C17" s="52"/>
-      <c r="D17" s="52"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="52"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="44"/>
+      <c r="E17" s="44"/>
+      <c r="F17" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3432,14 +3432,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="18.399999999999999" thickTop="1" thickBot="1">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="50"/>
-      <c r="C1" s="50"/>
-      <c r="D1" s="50"/>
-      <c r="E1" s="50"/>
-      <c r="F1" s="51"/>
+      <c r="B1" s="56"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="57"/>
     </row>
     <row r="2" spans="1:6" ht="13.9" thickTop="1" thickBot="1">
       <c r="A2" s="22"/>
@@ -3553,6 +3553,30 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Levels xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">L1</Levels>
+    <Category xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Module Artifact</Category>
+    <FolderName xmlns="952a6df7-b138-4f89-9bc4-e7a874ea3254" xsi:nil="true"/>
+    <Material_x0020_Type xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Extra Material</Material_x0020_Type>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010046351F880B96AE4B9BB4815879ADEBDD" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="487f15db4e05f84fdb19aa3f548b93b8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81372d4e-bcfc-4844-a57b-a09c5da71958" xmlns:ns3="952a6df7-b138-4f89-9bc4-e7a874ea3254" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="09419ac551552483846d59652a820d17" ns2:_="" ns3:_="">
     <xsd:import namespace="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
@@ -3722,31 +3746,40 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Levels xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">L1</Levels>
-    <Category xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Module Artifact</Category>
-    <FolderName xmlns="952a6df7-b138-4f89-9bc4-e7a874ea3254" xsi:nil="true"/>
-    <Material_x0020_Type xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Extra Material</Material_x0020_Type>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67F96C4C-21BE-4526-9614-87D2A1A52CD5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E4DBA88-91AD-42CE-827B-50AA920D4CEA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{812CC0C1-FD42-47A7-BEBF-6413B223EE92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="952a6df7-b138-4f89-9bc4-e7a874ea3254"/>
+    <ds:schemaRef ds:uri="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38E28044-843A-4D7D-9F1F-711CA3C23377}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3763,37 +3796,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{812CC0C1-FD42-47A7-BEBF-6413B223EE92}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="952a6df7-b138-4f89-9bc4-e7a874ea3254"/>
-    <ds:schemaRef ds:uri="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E4DBA88-91AD-42CE-827B-50AA920D4CEA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67F96C4C-21BE-4526-9614-87D2A1A52CD5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add employee ui test case design
</commit_message>
<xml_diff>
--- a/Test Template Document Corp.xlsx
+++ b/Test Template Document Corp.xlsx
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="155">
   <si>
     <t>Project ID</t>
   </si>
@@ -445,9 +445,6 @@
   </si>
   <si>
     <t>OH_Req 10</t>
-  </si>
-  <si>
-    <t>OH_Req 11</t>
   </si>
   <si>
     <t>OH_Req 12</t>
@@ -503,6 +500,105 @@
   </si>
   <si>
     <t>Any one for testing</t>
+  </si>
+  <si>
+    <t>1. Title is "OrangeHRM" as expected
+2. Logo is displayed properly
+3. Textbox for entering username and password</t>
+  </si>
+  <si>
+    <t>failed</t>
+  </si>
+  <si>
+    <t>3. Link not available for ""Forgot Your Password?""</t>
+  </si>
+  <si>
+    <t>OH_Req 6.3</t>
+  </si>
+  <si>
+    <t>Employee - Add</t>
+  </si>
+  <si>
+    <t>SC_OH_09</t>
+  </si>
+  <si>
+    <t>TC_OH_13</t>
+  </si>
+  <si>
+    <t>To verify UI component for add employee section</t>
+  </si>
+  <si>
+    <t>Data: 
+Add username: Admin
+password- admin123</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Navigate to the url
+2. Enter Admin username
+3. Enter password
+4. Click Login
+5. Mouse over on PIM
+6. Click on Add Employee
+</t>
+  </si>
+  <si>
+    <t>TC_OH_14</t>
+  </si>
+  <si>
+    <t>To verify UI component for add employee section after checking create login details</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Navigate to the url
+2. Enter Admin username
+3. Enter password
+4. Click Login
+5. Mouse over on PIM
+6. Click on Add Employee
+7. Check - Create Login Details
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Add Employee header should be displayed 
+2. Logo should be displayed
+3. Textbox for firstname, middle name, lastname, employee id
+4. Choose file option for Image upload should be provided 
+5. Checkbox for create login detail 
+6. Save button should be displayed 
+7. Label for firstname, lastname, middle name, emp photo, Employee id, create login detail should be displayed properly 
+8. For image upload the info should be displayed "Accepts jpg, .png, .gif up to 1MB. Recommended dimensions: 200px X 200px"
+ </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">1. Add Employee header should be displayed 
+2. Logo should be displayed
+3. Textbox for firstname, middle name, lastname, employee id
+4. Choose file option for Image upload should be provided 
+5. Checkbox for create login detail 
+6. Save button should be displayed 
+7. Label for firstname, lastname, middle name, emp photo, Employee id, create login detail should be displayed properly 
+8. For image upload the info should be displayed "Accepts jpg, .png, .gif up to 1MB. Recommended dimensions: 200px X 200px"
+9. Textbox for username, password, confirm password should be displayed
+10. Dropdown for status with option as </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>enabled</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+      </rPr>
+      <t xml:space="preserve"> and disabled should be available
+11. Label should be dispayed for username, password, confirm password, status.
+ </t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1009,7 +1105,7 @@
         <xdr:cNvPr id="2154" name="Picture 2" descr="pcs">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006A080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006A080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1566,7 +1662,7 @@
   <dimension ref="A2:D18"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="12.75"/>
@@ -1698,7 +1794,7 @@
         <v>63</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D13" s="15"/>
     </row>
@@ -1714,17 +1810,19 @@
     </row>
     <row r="15" spans="1:4" ht="13.9">
       <c r="A15" s="34" t="s">
-        <v>125</v>
+        <v>143</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="15"/>
+      <c r="C15" s="15" t="s">
+        <v>144</v>
+      </c>
       <c r="D15" s="31"/>
     </row>
     <row r="16" spans="1:4" ht="13.9">
       <c r="A16" s="34" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>66</v>
@@ -1734,7 +1832,7 @@
     </row>
     <row r="17" spans="1:4" ht="13.9">
       <c r="A17" s="34" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>67</v>
@@ -1744,7 +1842,7 @@
     </row>
     <row r="18" spans="1:4" ht="13.9">
       <c r="A18" s="34" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>68</v>
@@ -1767,8 +1865,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M387"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36" defaultRowHeight="12.75"/>
@@ -1876,6 +1974,15 @@
       <c r="G3" s="37" t="s">
         <v>75</v>
       </c>
+      <c r="H3" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>141</v>
+      </c>
+      <c r="J3" s="21" t="s">
+        <v>142</v>
+      </c>
       <c r="K3" s="40">
         <v>44607</v>
       </c>
@@ -2001,7 +2108,7 @@
         <v>97</v>
       </c>
       <c r="G8" s="42" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="K8" s="40"/>
     </row>
@@ -2111,27 +2218,66 @@
         <v>118</v>
       </c>
       <c r="C14" s="37" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="D14" s="37" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="E14" s="37" t="s">
         <v>97</v>
       </c>
       <c r="F14" s="32"/>
       <c r="G14" s="21" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="K14" s="40"/>
     </row>
-    <row r="15" spans="1:13" s="21" customFormat="1">
-      <c r="E15" s="32"/>
+    <row r="15" spans="1:13" s="21" customFormat="1" ht="153">
+      <c r="A15" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>146</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>147</v>
+      </c>
+      <c r="D15" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="E15" s="37" t="s">
+        <v>149</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>153</v>
+      </c>
       <c r="J15" s="40"/>
     </row>
-    <row r="16" spans="1:13" s="21" customFormat="1">
-      <c r="A16" s="33"/>
-      <c r="F16" s="32"/>
+    <row r="16" spans="1:13" s="21" customFormat="1" ht="229.9">
+      <c r="A16" s="21" t="s">
+        <v>145</v>
+      </c>
+      <c r="B16" s="37" t="s">
+        <v>150</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>151</v>
+      </c>
+      <c r="D16" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="E16" s="37" t="s">
+        <v>152</v>
+      </c>
+      <c r="F16" s="21" t="s">
+        <v>148</v>
+      </c>
+      <c r="G16" s="37" t="s">
+        <v>154</v>
+      </c>
       <c r="K16" s="40"/>
     </row>
     <row r="17" spans="1:11" s="21" customFormat="1">
@@ -3262,7 +3408,7 @@
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I3:J14 I16:J57 H15:I15">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I16:I57 H15:I15 I3:I14">
       <formula1>"passed,failed,skipped,blocked"</formula1>
     </dataValidation>
   </dataValidations>
@@ -3303,7 +3449,7 @@
   <sheetData>
     <row r="6" spans="3:6" ht="27.4">
       <c r="C6" s="44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D6" s="44"/>
       <c r="E6" s="44"/>
@@ -3324,25 +3470,25 @@
     <row r="9" spans="3:6" ht="27.4">
       <c r="C9" s="44"/>
       <c r="D9" s="44" t="s">
+        <v>134</v>
+      </c>
+      <c r="E9" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="E9" s="44" t="s">
-        <v>136</v>
-      </c>
       <c r="F9" s="44" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="10" spans="3:6" s="46" customFormat="1" ht="27.4">
       <c r="C10" s="45"/>
       <c r="D10" s="45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E10" s="45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F10" s="45" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="11" spans="3:6" s="48" customFormat="1" ht="27.4">
@@ -3354,7 +3500,7 @@
     <row r="12" spans="3:6" s="48" customFormat="1" ht="27.4">
       <c r="C12" s="47"/>
       <c r="D12" s="54" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E12" s="54"/>
       <c r="F12" s="54"/>
@@ -3362,37 +3508,37 @@
     <row r="13" spans="3:6" ht="27.4">
       <c r="C13" s="44"/>
       <c r="D13" s="44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E13" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="F13" s="44" t="s">
         <v>137</v>
-      </c>
-      <c r="F13" s="44" t="s">
-        <v>138</v>
       </c>
     </row>
     <row r="14" spans="3:6" ht="27.4">
       <c r="C14" s="44"/>
       <c r="D14" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="44" t="s">
         <v>137</v>
       </c>
-      <c r="E14" s="44" t="s">
-        <v>138</v>
-      </c>
       <c r="F14" s="44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="15" spans="3:6" ht="27.4">
       <c r="C15" s="44"/>
       <c r="D15" s="44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="E15" s="44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="F15" s="44" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="16" spans="3:6" ht="27.4">
@@ -3553,30 +3699,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Levels xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">L1</Levels>
-    <Category xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Module Artifact</Category>
-    <FolderName xmlns="952a6df7-b138-4f89-9bc4-e7a874ea3254" xsi:nil="true"/>
-    <Material_x0020_Type xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Extra Material</Material_x0020_Type>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010046351F880B96AE4B9BB4815879ADEBDD" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="487f15db4e05f84fdb19aa3f548b93b8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81372d4e-bcfc-4844-a57b-a09c5da71958" xmlns:ns3="952a6df7-b138-4f89-9bc4-e7a874ea3254" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="09419ac551552483846d59652a820d17" ns2:_="" ns3:_="">
     <xsd:import namespace="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
@@ -3746,23 +3868,50 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Levels xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">L1</Levels>
+    <Category xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Module Artifact</Category>
+    <FolderName xmlns="952a6df7-b138-4f89-9bc4-e7a874ea3254" xsi:nil="true"/>
+    <Material_x0020_Type xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Extra Material</Material_x0020_Type>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67F96C4C-21BE-4526-9614-87D2A1A52CD5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38E28044-843A-4D7D-9F1F-711CA3C23377}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
+    <ds:schemaRef ds:uri="952a6df7-b138-4f89-9bc4-e7a874ea3254"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E4DBA88-91AD-42CE-827B-50AA920D4CEA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{812CC0C1-FD42-47A7-BEBF-6413B223EE92}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -3779,21 +3928,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E4DBA88-91AD-42CE-827B-50AA920D4CEA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38E28044-843A-4D7D-9F1F-711CA3C23377}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67F96C4C-21BE-4526-9614-87D2A1A52CD5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
-    <ds:schemaRef ds:uri="952a6df7-b138-4f89-9bc4-e7a874ea3254"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add employee ui test case design2
</commit_message>
<xml_diff>
--- a/Test Template Document Corp.xlsx
+++ b/Test Template Document Corp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="5468" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="5468" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Project Profile" sheetId="6" r:id="rId1"/>
@@ -516,9 +516,6 @@
     <t>OH_Req 6.3</t>
   </si>
   <si>
-    <t>Employee - Add</t>
-  </si>
-  <si>
     <t>SC_OH_09</t>
   </si>
   <si>
@@ -594,11 +591,15 @@
       <rPr>
         <sz val="10"/>
         <rFont val="Arial"/>
+        <family val="2"/>
       </rPr>
       <t xml:space="preserve"> and disabled should be available
 11. Label should be dispayed for username, password, confirm password, status.
  </t>
     </r>
+  </si>
+  <si>
+    <t>Add Employee</t>
   </si>
 </sst>
 </file>
@@ -1105,7 +1106,7 @@
         <xdr:cNvPr id="2154" name="Picture 2" descr="pcs">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006A080000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006A080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1661,7 +1662,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D18"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -1815,8 +1816,8 @@
       <c r="B15" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="C15" s="15" t="s">
-        <v>144</v>
+      <c r="C15" s="36" t="s">
+        <v>154</v>
       </c>
       <c r="D15" s="31"/>
     </row>
@@ -1865,8 +1866,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M387"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36" defaultRowHeight="12.75"/>
@@ -2234,49 +2235,49 @@
     </row>
     <row r="15" spans="1:13" s="21" customFormat="1" ht="153">
       <c r="A15" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B15" s="37" t="s">
         <v>145</v>
       </c>
-      <c r="B15" s="37" t="s">
+      <c r="C15" s="21" t="s">
         <v>146</v>
-      </c>
-      <c r="C15" s="21" t="s">
-        <v>147</v>
       </c>
       <c r="D15" s="37" t="s">
         <v>129</v>
       </c>
       <c r="E15" s="37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G15" s="21" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="J15" s="40"/>
     </row>
     <row r="16" spans="1:13" s="21" customFormat="1" ht="229.9">
       <c r="A16" s="21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B16" s="37" t="s">
+        <v>149</v>
+      </c>
+      <c r="C16" s="21" t="s">
         <v>150</v>
-      </c>
-      <c r="C16" s="21" t="s">
-        <v>151</v>
       </c>
       <c r="D16" s="37" t="s">
         <v>129</v>
       </c>
       <c r="E16" s="37" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G16" s="37" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="K16" s="40"/>
     </row>
@@ -3699,6 +3700,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Levels xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">L1</Levels>
+    <Category xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Module Artifact</Category>
+    <FolderName xmlns="952a6df7-b138-4f89-9bc4-e7a874ea3254" xsi:nil="true"/>
+    <Material_x0020_Type xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Extra Material</Material_x0020_Type>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010046351F880B96AE4B9BB4815879ADEBDD" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="487f15db4e05f84fdb19aa3f548b93b8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81372d4e-bcfc-4844-a57b-a09c5da71958" xmlns:ns3="952a6df7-b138-4f89-9bc4-e7a874ea3254" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="09419ac551552483846d59652a820d17" ns2:_="" ns3:_="">
     <xsd:import namespace="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
@@ -3868,18 +3880,11 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Levels xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">L1</Levels>
-    <Category xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Module Artifact</Category>
-    <FolderName xmlns="952a6df7-b138-4f89-9bc4-e7a874ea3254" xsi:nil="true"/>
-    <Material_x0020_Type xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Extra Material</Material_x0020_Type>
-  </documentManagement>
-</p:properties>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -3888,11 +3893,24 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{812CC0C1-FD42-47A7-BEBF-6413B223EE92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="952a6df7-b138-4f89-9bc4-e7a874ea3254"/>
+    <ds:schemaRef ds:uri="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38E28044-843A-4D7D-9F1F-711CA3C23377}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3911,35 +3929,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{812CC0C1-FD42-47A7-BEBF-6413B223EE92}">
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67F96C4C-21BE-4526-9614-87D2A1A52CD5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="952a6df7-b138-4f89-9bc4-e7a874ea3254"/>
-    <ds:schemaRef ds:uri="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E4DBA88-91AD-42CE-827B-50AA920D4CEA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67F96C4C-21BE-4526-9614-87D2A1A52CD5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
TC-add employee without credential
</commit_message>
<xml_diff>
--- a/Test Template Document Corp.xlsx
+++ b/Test Template Document Corp.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="5468" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14385" windowHeight="5468" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Project Profile" sheetId="6" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="155">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="164">
   <si>
     <t>Project ID</t>
   </si>
@@ -555,11 +555,14 @@
 </t>
   </si>
   <si>
+    <t>Add Employee</t>
+  </si>
+  <si>
     <t xml:space="preserve">1. Add Employee header should be displayed 
 2. Logo should be displayed
 3. Textbox for firstname, middle name, lastname, employee id
 4. Choose file option for Image upload should be provided 
-5. Checkbox for create login detail 
+5. Checkbox for create login detail should be displayed and should be unchecked
 6. Save button should be displayed 
 7. Label for firstname, lastname, middle name, emp photo, Employee id, create login detail should be displayed properly 
 8. For image upload the info should be displayed "Accepts jpg, .png, .gif up to 1MB. Recommended dimensions: 200px X 200px"
@@ -571,7 +574,7 @@
 2. Logo should be displayed
 3. Textbox for firstname, middle name, lastname, employee id
 4. Choose file option for Image upload should be provided 
-5. Checkbox for create login detail 
+5. Checkbox for create login detail should be displayed and should be checked
 6. Save button should be displayed 
 7. Label for firstname, lastname, middle name, emp photo, Employee id, create login detail should be displayed properly 
 8. For image upload the info should be displayed "Accepts jpg, .png, .gif up to 1MB. Recommended dimensions: 200px X 200px"
@@ -593,13 +596,75 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> and disabled should be available
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>disabled</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> should be available and in that enabled should be selected.
 11. Label should be dispayed for username, password, confirm password, status.
  </t>
     </r>
   </si>
   <si>
-    <t>Add Employee</t>
+    <t>TC_OH_15</t>
+  </si>
+  <si>
+    <t>To verify the valid record of add employee without providing credentials</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Navigate to the url
+2. Enter Admin username
+3. Enter password
+4. Click Login
+5. Mouse over on PIM
+6. Click on Add Employee
+7. Enter firstname
+8. Enter middlename
+9. Enter lastname
+10. Enter Employee Id
+11. Upload the employee image
+12. Click on save
+</t>
+  </si>
+  <si>
+    <t>Data:
+1. Username: Admin
+2. Password: admin123
+3. Firstname: John
+4. MiddleName: J
+5. Last Name: Wick
+6.Employee Id: 4545
+7.Upload image: "C:\Users\JiDi\Pictures\Screenshots\Screenshot (1).png"</t>
+  </si>
+  <si>
+    <t>1. Admin should see message as "Employee record has been added to employee list"
+2. The added employee details should be present in the employee list.(PIM--&gt;EmployeeList)
+3. Database should contains the added employee details.</t>
+  </si>
+  <si>
+    <t>TC_OH_16</t>
+  </si>
+  <si>
+    <t>To verify the valid record of add employee by providing credentials with enabled mode</t>
+  </si>
+  <si>
+    <t>TC_OH_17</t>
+  </si>
+  <si>
+    <t>To verify the valid record of add employee by providing credentials with disabled mode</t>
   </si>
 </sst>
 </file>
@@ -1106,7 +1171,7 @@
         <xdr:cNvPr id="2154" name="Picture 2" descr="pcs">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00006A080000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-00006A080000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1662,7 +1727,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
@@ -1817,7 +1882,7 @@
         <v>65</v>
       </c>
       <c r="C15" s="36" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D15" s="31"/>
     </row>
@@ -1866,8 +1931,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M387"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" topLeftCell="A17" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="36" defaultRowHeight="12.75"/>
@@ -1876,7 +1941,7 @@
     <col min="2" max="2" width="18.265625" style="1" customWidth="1"/>
     <col min="3" max="3" width="35.3984375" style="1" customWidth="1"/>
     <col min="4" max="4" width="38.59765625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="25.265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="34.59765625" style="1" customWidth="1"/>
     <col min="6" max="6" width="33.73046875" style="1" customWidth="1"/>
     <col min="7" max="7" width="57.9296875" style="1" customWidth="1"/>
     <col min="8" max="10" width="26.1328125" style="1" customWidth="1"/>
@@ -2233,7 +2298,7 @@
       </c>
       <c r="K14" s="40"/>
     </row>
-    <row r="15" spans="1:13" s="21" customFormat="1" ht="153">
+    <row r="15" spans="1:13" s="21" customFormat="1" ht="165.75">
       <c r="A15" s="21" t="s">
         <v>144</v>
       </c>
@@ -2253,11 +2318,11 @@
         <v>147</v>
       </c>
       <c r="G15" s="21" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="J15" s="40"/>
     </row>
-    <row r="16" spans="1:13" s="21" customFormat="1" ht="229.9">
+    <row r="16" spans="1:13" s="21" customFormat="1" ht="242.65">
       <c r="A16" s="21" t="s">
         <v>144</v>
       </c>
@@ -2277,21 +2342,57 @@
         <v>147</v>
       </c>
       <c r="G16" s="37" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="K16" s="40"/>
     </row>
-    <row r="17" spans="1:11" s="21" customFormat="1">
-      <c r="A17" s="33"/>
-      <c r="F17" s="32"/>
+    <row r="17" spans="1:11" s="21" customFormat="1" ht="161.25" customHeight="1">
+      <c r="A17" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B17" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="D17" s="37" t="s">
+        <v>129</v>
+      </c>
+      <c r="E17" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="F17" s="42" t="s">
+        <v>158</v>
+      </c>
+      <c r="G17" s="37" t="s">
+        <v>159</v>
+      </c>
       <c r="K17" s="40"/>
     </row>
-    <row r="18" spans="1:11" s="21" customFormat="1">
-      <c r="A18" s="33"/>
+    <row r="18" spans="1:11" s="21" customFormat="1" ht="38.25">
+      <c r="A18" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B18" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>161</v>
+      </c>
       <c r="F18" s="32"/>
       <c r="K18" s="40"/>
     </row>
-    <row r="19" spans="1:11" s="21" customFormat="1">
+    <row r="19" spans="1:11" s="21" customFormat="1" ht="38.25">
+      <c r="A19" s="21" t="s">
+        <v>144</v>
+      </c>
+      <c r="B19" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="C19" s="37" t="s">
+        <v>163</v>
+      </c>
       <c r="F19" s="32"/>
       <c r="K19" s="40"/>
     </row>
@@ -3700,17 +3801,19 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Levels xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">L1</Levels>
-    <Category xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Module Artifact</Category>
-    <FolderName xmlns="952a6df7-b138-4f89-9bc4-e7a874ea3254" xsi:nil="true"/>
-    <Material_x0020_Type xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Extra Material</Material_x0020_Type>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010046351F880B96AE4B9BB4815879ADEBDD" ma:contentTypeVersion="3" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="487f15db4e05f84fdb19aa3f548b93b8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="81372d4e-bcfc-4844-a57b-a09c5da71958" xmlns:ns3="952a6df7-b138-4f89-9bc4-e7a874ea3254" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="09419ac551552483846d59652a820d17" ns2:_="" ns3:_="">
     <xsd:import namespace="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
@@ -3880,37 +3983,34 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<LongProperties xmlns="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-</file>
-
 <file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Levels xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">L1</Levels>
+    <Category xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Module Artifact</Category>
+    <FolderName xmlns="952a6df7-b138-4f89-9bc4-e7a874ea3254" xsi:nil="true"/>
+    <Material_x0020_Type xmlns="81372d4e-bcfc-4844-a57b-a09c5da71958">Extra Material</Material_x0020_Type>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{812CC0C1-FD42-47A7-BEBF-6413B223EE92}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E4DBA88-91AD-42CE-827B-50AA920D4CEA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="952a6df7-b138-4f89-9bc4-e7a874ea3254"/>
-    <ds:schemaRef ds:uri="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67F96C4C-21BE-4526-9614-87D2A1A52CD5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38E28044-843A-4D7D-9F1F-711CA3C23377}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3929,18 +4029,19 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67F96C4C-21BE-4526-9614-87D2A1A52CD5}">
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{812CC0C1-FD42-47A7-BEBF-6413B223EE92}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/longProperties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3E4DBA88-91AD-42CE-827B-50AA920D4CEA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="952a6df7-b138-4f89-9bc4-e7a874ea3254"/>
+    <ds:schemaRef ds:uri="81372d4e-bcfc-4844-a57b-a09c5da71958"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>